<commit_message>
half of the required changes
</commit_message>
<xml_diff>
--- a/client/dist/pyreport/report3.xlsx
+++ b/client/dist/pyreport/report3.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="33465" yWindow="1365" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="1" state="visible" r:id="rId1"/>
@@ -90,17 +90,16 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Summary'!$2:$6</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Summary'!$B$1:$U$51</definedName>
   </definedNames>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="181029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="[$-409]mmm\-yy;@"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="17">
     <font>
@@ -632,38 +631,10 @@
       <right style="double">
         <color indexed="64"/>
       </right>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top style="double">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -683,6 +654,49 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -697,21 +711,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -722,7 +721,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="166" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="96">
@@ -823,40 +822,13 @@
     <xf numFmtId="2" fontId="11" fillId="0" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
@@ -866,6 +838,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
@@ -892,10 +876,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
@@ -904,7 +903,7 @@
     <xf numFmtId="164" fontId="11" fillId="0" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="34" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="37" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -913,31 +912,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="34" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="37" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="34" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="37" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="33" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="38" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="35" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="36" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="35" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="36" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="39" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="33" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="39" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="33" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3899,7 +3898,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4203,12 +4202,12 @@
   <dimension ref="A1:W81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M160" sqref="M160"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="U84" sqref="U84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
     <col width="2.7109375" customWidth="1" style="2" min="1" max="1"/>
     <col width="8.7109375" customWidth="1" style="2" min="2" max="6"/>
@@ -4271,7 +4270,7 @@
         </is>
       </c>
       <c r="C3" s="6" t="n"/>
-      <c r="D3" s="67" t="inlineStr">
+      <c r="D3" s="62" t="inlineStr">
         <is>
           <t>ROSSING</t>
         </is>
@@ -4318,7 +4317,7 @@
           <t>Period:</t>
         </is>
       </c>
-      <c r="M4" s="68" t="n"/>
+      <c r="M4" s="63" t="n"/>
       <c r="N4" s="80" t="n"/>
       <c r="O4" s="80" t="n"/>
       <c r="P4" s="12" t="n"/>
@@ -4343,15 +4342,15 @@
         </is>
       </c>
       <c r="L5" s="8" t="n"/>
-      <c r="M5" s="69" t="n">
-        <v>45145</v>
+      <c r="M5" s="64" t="n">
+        <v>45154</v>
       </c>
       <c r="N5" s="81" t="n"/>
       <c r="O5" s="81" t="n"/>
       <c r="P5" s="81" t="n"/>
       <c r="Q5" s="8" t="n"/>
       <c r="R5" s="9" t="n"/>
-      <c r="S5" s="71" t="n"/>
+      <c r="S5" s="66" t="n"/>
       <c r="U5" s="82" t="n"/>
     </row>
     <row r="6" ht="6.75" customHeight="1" thickBot="1" thickTop="1">
@@ -4621,31 +4620,31 @@
       </c>
       <c r="F14" s="91" t="n"/>
       <c r="G14" s="41" t="n">
-        <v>-5.174134</v>
+        <v>-5.886086</v>
       </c>
       <c r="H14" s="42" t="n">
-        <v>-4.11092</v>
+        <v>-4.291172</v>
       </c>
       <c r="I14" s="43" t="n">
-        <v>-4.69540709009009</v>
+        <v>-5.037621084626234</v>
       </c>
       <c r="J14" s="41" t="n">
-        <v>-5.174134</v>
+        <v>-5.886086</v>
       </c>
       <c r="K14" s="42" t="n">
-        <v>-3.671011</v>
+        <v>-4.019265</v>
       </c>
       <c r="L14" s="43" t="n">
-        <v>-4.548637083216783</v>
+        <v>-4.820824186947655</v>
       </c>
       <c r="M14" s="41" t="n">
-        <v>-5.174134</v>
+        <v>-5.886086</v>
       </c>
       <c r="N14" s="42" t="n">
         <v>-3.457166</v>
       </c>
       <c r="O14" s="43" t="n">
-        <v>-4.358037545278638</v>
+        <v>-4.483940334441489</v>
       </c>
       <c r="P14" s="92" t="n">
         <v>21.047</v>
@@ -4673,31 +4672,31 @@
       </c>
       <c r="F15" s="91" t="n"/>
       <c r="G15" s="44" t="n">
-        <v>-22.987986</v>
+        <v>-24.193577</v>
       </c>
       <c r="H15" s="42" t="n">
-        <v>-20.916549</v>
+        <v>-21.688834</v>
       </c>
       <c r="I15" s="45" t="n">
-        <v>-21.89715079939668</v>
+        <v>-22.96590238801712</v>
       </c>
       <c r="J15" s="44" t="n">
-        <v>-22.987986</v>
+        <v>-24.193577</v>
       </c>
       <c r="K15" s="42" t="n">
-        <v>-18.910349</v>
+        <v>-19.650094</v>
       </c>
       <c r="L15" s="45" t="n">
-        <v>-21.0094540190007</v>
+        <v>-21.97064139041096</v>
       </c>
       <c r="M15" s="44" t="n">
-        <v>-22.987986</v>
+        <v>-24.193577</v>
       </c>
       <c r="N15" s="42" t="n">
         <v>-17.644213</v>
       </c>
       <c r="O15" s="45" t="n">
-        <v>-20.43971266614502</v>
+        <v>-20.96838347837259</v>
       </c>
       <c r="P15" s="92" t="n">
         <v>22.912</v>
@@ -4725,22 +4724,22 @@
       </c>
       <c r="F16" s="91" t="n"/>
       <c r="G16" s="44" t="n">
-        <v>135.738596</v>
+        <v>136.097429</v>
       </c>
       <c r="H16" s="42" t="n">
         <v>136.981793</v>
       </c>
       <c r="I16" s="45" t="n">
-        <v>136.2579085656108</v>
+        <v>136.4433245663338</v>
       </c>
       <c r="J16" s="44" t="n">
-        <v>135.382405</v>
+        <v>135.606231</v>
       </c>
       <c r="K16" s="42" t="n">
         <v>136.981793</v>
       </c>
       <c r="L16" s="45" t="n">
-        <v>135.9718815102041</v>
+        <v>136.1531335993151</v>
       </c>
       <c r="M16" s="44" t="n">
         <v>134.833634</v>
@@ -4749,7 +4748,7 @@
         <v>136.981793</v>
       </c>
       <c r="O16" s="45" t="n">
-        <v>135.7868104580073</v>
+        <v>135.8759337940043</v>
       </c>
       <c r="P16" s="92" t="n">
         <v>34.487</v>
@@ -4777,22 +4776,22 @@
       </c>
       <c r="F17" s="91" t="n"/>
       <c r="G17" s="44" t="n">
-        <v>-9.751659999999999</v>
+        <v>-9.833931</v>
       </c>
       <c r="H17" s="42" t="n">
         <v>-8.400447</v>
       </c>
       <c r="I17" s="45" t="n">
-        <v>-9.014780848575713</v>
+        <v>-9.139304539660056</v>
       </c>
       <c r="J17" s="44" t="n">
-        <v>-10.837253</v>
+        <v>-9.833931</v>
       </c>
       <c r="K17" s="42" t="n">
         <v>-8.400447</v>
       </c>
       <c r="L17" s="45" t="n">
-        <v>-9.2134480174703</v>
+        <v>-9.148182310626703</v>
       </c>
       <c r="M17" s="44" t="n">
         <v>-13.524911</v>
@@ -4801,7 +4800,7 @@
         <v>-8.400447</v>
       </c>
       <c r="O17" s="45" t="n">
-        <v>-9.80874214919044</v>
+        <v>-9.737134997014925</v>
       </c>
       <c r="P17" s="92" t="n">
         <v>6.957</v>
@@ -4829,31 +4828,31 @@
       </c>
       <c r="F18" s="91" t="n"/>
       <c r="G18" s="44" t="n">
-        <v>22.538347</v>
+        <v>22.178889</v>
       </c>
       <c r="H18" s="42" t="n">
-        <v>23.221274</v>
+        <v>23.2063</v>
       </c>
       <c r="I18" s="45" t="n">
-        <v>22.88432981818182</v>
+        <v>22.70635168554396</v>
       </c>
       <c r="J18" s="44" t="n">
-        <v>22.538347</v>
+        <v>22.178889</v>
       </c>
       <c r="K18" s="42" t="n">
-        <v>23.520781</v>
+        <v>23.251242</v>
       </c>
       <c r="L18" s="45" t="n">
-        <v>22.95006179063165</v>
+        <v>22.82000633962264</v>
       </c>
       <c r="M18" s="44" t="n">
-        <v>22.538347</v>
+        <v>22.178889</v>
       </c>
       <c r="N18" s="42" t="n">
         <v>24.574957</v>
       </c>
       <c r="O18" s="45" t="n">
-        <v>23.29328154577192</v>
+        <v>23.19996823724832</v>
       </c>
       <c r="P18" s="92" t="n">
         <v>24.746</v>
@@ -4881,31 +4880,31 @@
       </c>
       <c r="F19" s="91" t="n"/>
       <c r="G19" s="44" t="n">
-        <v>-3.748356</v>
+        <v>-4.280219</v>
       </c>
       <c r="H19" s="42" t="n">
-        <v>-2.514851</v>
+        <v>-2.920743</v>
       </c>
       <c r="I19" s="45" t="n">
-        <v>-3.245554170658683</v>
+        <v>-3.605624666195191</v>
       </c>
       <c r="J19" s="44" t="n">
-        <v>-3.748356</v>
+        <v>-4.280219</v>
       </c>
       <c r="K19" s="42" t="n">
-        <v>-2.294588</v>
+        <v>-2.467644</v>
       </c>
       <c r="L19" s="45" t="n">
-        <v>-3.094284892382949</v>
+        <v>-3.37158197479564</v>
       </c>
       <c r="M19" s="44" t="n">
-        <v>-3.748356</v>
+        <v>-4.280219</v>
       </c>
       <c r="N19" s="42" t="n">
         <v>-2.014555</v>
       </c>
       <c r="O19" s="45" t="n">
-        <v>-2.893455135470942</v>
+        <v>-3.02600807890223</v>
       </c>
       <c r="P19" s="92" t="n">
         <v>8.914999999999999</v>
@@ -4933,31 +4932,31 @@
       </c>
       <c r="F20" s="91" t="n"/>
       <c r="G20" s="44" t="n">
-        <v>58.675162</v>
+        <v>67.370591</v>
       </c>
       <c r="H20" s="42" t="n">
-        <v>71.707238</v>
+        <v>76.16544</v>
       </c>
       <c r="I20" s="45" t="n">
-        <v>65.95142466666667</v>
+        <v>72.0575305</v>
       </c>
       <c r="J20" s="44" t="n">
-        <v>37.718299</v>
+        <v>46.865184</v>
       </c>
       <c r="K20" s="42" t="n">
-        <v>71.707238</v>
+        <v>76.16544</v>
       </c>
       <c r="L20" s="45" t="n">
-        <v>55.99991613772455</v>
+        <v>64.70357462804878</v>
       </c>
       <c r="M20" s="44" t="n">
-        <v>32.925255</v>
+        <v>32.923854</v>
       </c>
       <c r="N20" s="42" t="n">
-        <v>71.707238</v>
+        <v>76.16544</v>
       </c>
       <c r="O20" s="45" t="n">
-        <v>42.20090940562249</v>
+        <v>45.463486536</v>
       </c>
       <c r="P20" s="92" t="n">
         <v>7.67999</v>
@@ -4985,31 +4984,31 @@
       </c>
       <c r="F21" s="91" t="n"/>
       <c r="G21" s="44" t="n">
-        <v>61.472286</v>
+        <v>61.284878</v>
       </c>
       <c r="H21" s="42" t="n">
-        <v>61.847235</v>
+        <v>61.659869</v>
       </c>
       <c r="I21" s="45" t="n">
-        <v>61.59901506756757</v>
+        <v>61.45718586486486</v>
       </c>
       <c r="J21" s="44" t="n">
-        <v>61.472286</v>
+        <v>61.284878</v>
       </c>
       <c r="K21" s="42" t="n">
-        <v>62.223669</v>
+        <v>62.034719</v>
       </c>
       <c r="L21" s="45" t="n">
-        <v>61.76460589610389</v>
+        <v>61.58033337341772</v>
       </c>
       <c r="M21" s="44" t="n">
-        <v>61.472286</v>
+        <v>61.284878</v>
       </c>
       <c r="N21" s="42" t="n">
-        <v>62.669661</v>
+        <v>62.598433</v>
       </c>
       <c r="O21" s="45" t="n">
-        <v>62.14485498901099</v>
+        <v>62.03056272903225</v>
       </c>
       <c r="P21" s="92" t="n">
         <v>41.35799</v>
@@ -5037,31 +5036,31 @@
       </c>
       <c r="F22" s="91" t="n"/>
       <c r="G22" s="44" t="n">
-        <v>-11.609795</v>
+        <v>-12.130511</v>
       </c>
       <c r="H22" s="42" t="n">
-        <v>-10.353252</v>
+        <v>-10.670259</v>
       </c>
       <c r="I22" s="45" t="n">
-        <v>-11.05342833532934</v>
+        <v>-11.42230112305516</v>
       </c>
       <c r="J22" s="44" t="n">
-        <v>-11.609795</v>
+        <v>-12.130511</v>
       </c>
       <c r="K22" s="42" t="n">
-        <v>-10.004242</v>
+        <v>-10.265985</v>
       </c>
       <c r="L22" s="45" t="n">
-        <v>-10.91925634032145</v>
+        <v>-11.19305488147139</v>
       </c>
       <c r="M22" s="44" t="n">
-        <v>-11.609795</v>
+        <v>-12.130511</v>
       </c>
       <c r="N22" s="42" t="n">
         <v>-9.759931</v>
       </c>
       <c r="O22" s="45" t="n">
-        <v>-10.68015684088176</v>
+        <v>-10.81784653893654</v>
       </c>
       <c r="P22" s="92" t="n">
         <v>7.086</v>
@@ -5089,31 +5088,31 @@
       </c>
       <c r="F23" s="91" t="n"/>
       <c r="G23" s="44" t="n">
-        <v>-4.181771</v>
+        <v>-4.318845</v>
       </c>
       <c r="H23" s="42" t="n">
+        <v>-3.49735</v>
+      </c>
+      <c r="I23" s="45" t="n">
+        <v>-3.886652868421053</v>
+      </c>
+      <c r="J23" s="44" t="n">
+        <v>-4.318845</v>
+      </c>
+      <c r="K23" s="42" t="n">
         <v>-3.362435</v>
       </c>
-      <c r="I23" s="45" t="n">
-        <v>-3.758141525</v>
-      </c>
-      <c r="J23" s="44" t="n">
-        <v>-4.181771</v>
-      </c>
-      <c r="K23" s="42" t="n">
-        <v>-3.361921</v>
-      </c>
       <c r="L23" s="45" t="n">
-        <v>-3.760868295454546</v>
+        <v>-3.840912894117647</v>
       </c>
       <c r="M23" s="44" t="n">
-        <v>-4.183427</v>
+        <v>-4.320767</v>
       </c>
       <c r="N23" s="42" t="n">
         <v>-3.361921</v>
       </c>
       <c r="O23" s="45" t="n">
-        <v>-3.793514602189781</v>
+        <v>-3.871074357933579</v>
       </c>
       <c r="P23" s="92" t="n">
         <v>26.31499</v>
@@ -5141,31 +5140,31 @@
       </c>
       <c r="F24" s="91" t="n"/>
       <c r="G24" s="44" t="n">
-        <v>79.072305</v>
+        <v>78.27391799999999</v>
       </c>
       <c r="H24" s="42" t="n">
-        <v>80.23035400000001</v>
+        <v>79.88642</v>
       </c>
       <c r="I24" s="45" t="n">
-        <v>79.69078831988041</v>
+        <v>79.03263034887006</v>
       </c>
       <c r="J24" s="44" t="n">
-        <v>79.072305</v>
+        <v>78.27391799999999</v>
       </c>
       <c r="K24" s="42" t="n">
-        <v>81.549043</v>
+        <v>80.90548699999999</v>
       </c>
       <c r="L24" s="45" t="n">
-        <v>80.28153053974896</v>
+        <v>79.62877123489477</v>
       </c>
       <c r="M24" s="44" t="n">
-        <v>79.072305</v>
+        <v>78.27391799999999</v>
       </c>
       <c r="N24" s="42" t="n">
         <v>157.524381</v>
       </c>
       <c r="O24" s="45" t="n">
-        <v>81.31242606925741</v>
+        <v>80.95715137185431</v>
       </c>
       <c r="P24" s="92" t="n">
         <v>14.03</v>
@@ -5193,31 +5192,31 @@
       </c>
       <c r="F25" s="91" t="n"/>
       <c r="G25" s="44" t="n">
-        <v>4.91491</v>
+        <v>4.717378</v>
       </c>
       <c r="H25" s="42" t="n">
-        <v>7.258358</v>
+        <v>7.027388</v>
       </c>
       <c r="I25" s="45" t="n">
-        <v>6.371907202985074</v>
+        <v>5.822675064880113</v>
       </c>
       <c r="J25" s="44" t="n">
-        <v>4.91491</v>
+        <v>4.717378</v>
       </c>
       <c r="K25" s="42" t="n">
-        <v>8.423093</v>
+        <v>7.941151</v>
       </c>
       <c r="L25" s="45" t="n">
-        <v>6.901376184411969</v>
+        <v>6.326390662143826</v>
       </c>
       <c r="M25" s="44" t="n">
-        <v>4.91491</v>
+        <v>4.717378</v>
       </c>
       <c r="N25" s="42" t="n">
         <v>12.90971</v>
       </c>
       <c r="O25" s="45" t="n">
-        <v>7.319236404749874</v>
+        <v>7.015534895833333</v>
       </c>
       <c r="P25" s="92" t="n">
         <v>10.102</v>
@@ -5245,22 +5244,22 @@
       </c>
       <c r="F26" s="91" t="n"/>
       <c r="G26" s="44" t="n">
-        <v>-24.271414</v>
+        <v>-24.622864</v>
       </c>
       <c r="H26" s="42" t="n">
-        <v>838.032889</v>
+        <v>832.3451700000001</v>
       </c>
       <c r="I26" s="45" t="n">
-        <v>58.09491553333334</v>
+        <v>21.059996125</v>
       </c>
       <c r="J26" s="44" t="n">
-        <v>-26.028263</v>
+        <v>-24.622864</v>
       </c>
       <c r="K26" s="42" t="n">
         <v>838.032889</v>
       </c>
       <c r="L26" s="45" t="n">
-        <v>57.62556545341615</v>
+        <v>45.61420231515152</v>
       </c>
       <c r="M26" s="44" t="n">
         <v>-26.378983</v>
@@ -5269,7 +5268,7 @@
         <v>841.252787</v>
       </c>
       <c r="O26" s="45" t="n">
-        <v>51.82691168377823</v>
+        <v>45.024470084</v>
       </c>
       <c r="P26" s="92" t="n">
         <v>17.94499</v>
@@ -5297,31 +5296,31 @@
       </c>
       <c r="F27" s="91" t="n"/>
       <c r="G27" s="44" t="n">
-        <v>15.304317</v>
+        <v>14.711709</v>
       </c>
       <c r="H27" s="42" t="n">
-        <v>18.461884</v>
+        <v>17.67368</v>
       </c>
       <c r="I27" s="45" t="n">
-        <v>16.96424284146341</v>
+        <v>16.30261797752809</v>
       </c>
       <c r="J27" s="44" t="n">
-        <v>13.330786</v>
+        <v>14.711709</v>
       </c>
       <c r="K27" s="42" t="n">
         <v>18.461884</v>
       </c>
       <c r="L27" s="45" t="n">
-        <v>16.22324696045198</v>
+        <v>16.59314749180328</v>
       </c>
       <c r="M27" s="44" t="n">
-        <v>-14.405589</v>
+        <v>-13.810717</v>
       </c>
       <c r="N27" s="42" t="n">
         <v>18.461884</v>
       </c>
       <c r="O27" s="45" t="n">
-        <v>2.798103713733076</v>
+        <v>5.340168231638418</v>
       </c>
       <c r="P27" s="92" t="n">
         <v>40.658</v>
@@ -5349,31 +5348,31 @@
       </c>
       <c r="F28" s="91" t="n"/>
       <c r="G28" s="44" t="n">
-        <v>-4.047284</v>
+        <v>-4.239745</v>
       </c>
       <c r="H28" s="42" t="n">
-        <v>-3.201482</v>
+        <v>-3.401623</v>
       </c>
       <c r="I28" s="45" t="n">
-        <v>-3.652373405063291</v>
+        <v>-3.85261069047619</v>
       </c>
       <c r="J28" s="44" t="n">
-        <v>-4.082767</v>
+        <v>-4.239745</v>
       </c>
       <c r="K28" s="42" t="n">
         <v>-3.201482</v>
       </c>
       <c r="L28" s="45" t="n">
-        <v>-3.667834494186046</v>
+        <v>-3.77707532</v>
       </c>
       <c r="M28" s="44" t="n">
-        <v>-4.542823</v>
+        <v>-4.239745</v>
       </c>
       <c r="N28" s="42" t="n">
         <v>-3.201482</v>
       </c>
       <c r="O28" s="45" t="n">
-        <v>-3.815526977596741</v>
+        <v>-3.750266758</v>
       </c>
       <c r="P28" s="92" t="n">
         <v>2</v>
@@ -5396,39 +5395,39 @@
       <c r="D29" s="91" t="n"/>
       <c r="E29" s="90" t="inlineStr">
         <is>
-          <t>ST-23-01</t>
+          <t>VW-10</t>
         </is>
       </c>
       <c r="F29" s="91" t="n"/>
       <c r="G29" s="44" t="n">
-        <v>-1.418376</v>
+        <v>-5.939956</v>
       </c>
       <c r="H29" s="42" t="n">
-        <v>-1.020371</v>
+        <v>-5.244905</v>
       </c>
       <c r="I29" s="45" t="n">
-        <v>-1.250603</v>
+        <v>-5.603133315789473</v>
       </c>
       <c r="J29" s="44" t="n">
-        <v>-1.702266</v>
+        <v>-5.939956</v>
       </c>
       <c r="K29" s="42" t="n">
-        <v>-1.020371</v>
+        <v>-4.969554</v>
       </c>
       <c r="L29" s="45" t="n">
-        <v>-1.371031166666667</v>
+        <v>-5.524639188235295</v>
       </c>
       <c r="M29" s="44" t="n">
-        <v>-1.702266</v>
+        <v>-5.941624</v>
       </c>
       <c r="N29" s="42" t="n">
-        <v>1669.721304</v>
+        <v>-4.969554</v>
       </c>
       <c r="O29" s="45" t="n">
-        <v>543.4810550555555</v>
+        <v>-5.561414177121772</v>
       </c>
       <c r="P29" s="92" t="n">
-        <v>10.009</v>
+        <v>23.67999</v>
       </c>
       <c r="Q29" s="91" t="n"/>
       <c r="R29" s="33" t="n"/>
@@ -5448,39 +5447,39 @@
       <c r="D30" s="91" t="n"/>
       <c r="E30" s="90" t="inlineStr">
         <is>
-          <t>VW-10</t>
+          <t>VW-ST-08</t>
         </is>
       </c>
       <c r="F30" s="91" t="n"/>
       <c r="G30" s="44" t="n">
-        <v>-5.66337</v>
+        <v>37.907629</v>
       </c>
       <c r="H30" s="42" t="n">
-        <v>-4.969554</v>
+        <v>39.25096</v>
       </c>
       <c r="I30" s="45" t="n">
-        <v>-5.443395</v>
+        <v>38.57894971590909</v>
       </c>
       <c r="J30" s="44" t="n">
-        <v>-5.66337</v>
+        <v>37.907629</v>
       </c>
       <c r="K30" s="42" t="n">
-        <v>-4.969554</v>
+        <v>39.633894</v>
       </c>
       <c r="L30" s="45" t="n">
-        <v>-5.437946556818182</v>
+        <v>38.82379366666667</v>
       </c>
       <c r="M30" s="44" t="n">
-        <v>-5.941227</v>
+        <v>37.720579</v>
       </c>
       <c r="N30" s="42" t="n">
-        <v>-4.969554</v>
+        <v>39.832263</v>
       </c>
       <c r="O30" s="45" t="n">
-        <v>-5.475070408759124</v>
+        <v>38.91059024902724</v>
       </c>
       <c r="P30" s="92" t="n">
-        <v>23.67999</v>
+        <v>9.787990000000001</v>
       </c>
       <c r="Q30" s="91" t="n"/>
       <c r="R30" s="33" t="n"/>
@@ -5500,39 +5499,39 @@
       <c r="D31" s="91" t="n"/>
       <c r="E31" s="90" t="inlineStr">
         <is>
-          <t>VW-ST-08</t>
+          <t>VW-ST-03</t>
         </is>
       </c>
       <c r="F31" s="91" t="n"/>
       <c r="G31" s="44" t="n">
-        <v>38.482542</v>
+        <v>-23.956972</v>
       </c>
       <c r="H31" s="42" t="n">
-        <v>39.633894</v>
+        <v>-23.203799</v>
       </c>
       <c r="I31" s="45" t="n">
-        <v>38.95948381012659</v>
+        <v>-23.55478687654321</v>
       </c>
       <c r="J31" s="44" t="n">
-        <v>38.482542</v>
+        <v>-23.956972</v>
       </c>
       <c r="K31" s="42" t="n">
-        <v>39.828603</v>
+        <v>-23.015539</v>
       </c>
       <c r="L31" s="45" t="n">
-        <v>39.07180865497076</v>
+        <v>-23.42539365644172</v>
       </c>
       <c r="M31" s="44" t="n">
-        <v>37.720579</v>
+        <v>-23.956972</v>
       </c>
       <c r="N31" s="42" t="n">
-        <v>39.832263</v>
+        <v>-22.63756</v>
       </c>
       <c r="O31" s="45" t="n">
-        <v>38.94132535059761</v>
+        <v>-23.18366132340426</v>
       </c>
       <c r="P31" s="92" t="n">
-        <v>9.787990000000001</v>
+        <v>11.36</v>
       </c>
       <c r="Q31" s="91" t="n"/>
       <c r="R31" s="33" t="n"/>
@@ -5546,45 +5545,45 @@
       <c r="B32" s="16" t="n"/>
       <c r="C32" s="90" t="inlineStr">
         <is>
-          <t>SILT-TRAP</t>
+          <t>E1/E2</t>
         </is>
       </c>
       <c r="D32" s="91" t="n"/>
       <c r="E32" s="90" t="inlineStr">
         <is>
-          <t>VW-ST-03</t>
+          <t>E2-7</t>
         </is>
       </c>
       <c r="F32" s="91" t="n"/>
       <c r="G32" s="44" t="n">
-        <v>-23.579963</v>
+        <v>0.490875</v>
       </c>
       <c r="H32" s="42" t="n">
-        <v>-23.015826</v>
+        <v>1.616566</v>
       </c>
       <c r="I32" s="45" t="n">
-        <v>-23.32830312676056</v>
+        <v>1.041660580872011</v>
       </c>
       <c r="J32" s="44" t="n">
-        <v>-23.579963</v>
+        <v>0.490875</v>
       </c>
       <c r="K32" s="42" t="n">
-        <v>-22.827324</v>
+        <v>2.323522</v>
       </c>
       <c r="L32" s="45" t="n">
-        <v>-23.25984863057325</v>
+        <v>1.37983298037889</v>
       </c>
       <c r="M32" s="44" t="n">
-        <v>-23.579963</v>
+        <v>0.490875</v>
       </c>
       <c r="N32" s="42" t="n">
-        <v>-22.63756</v>
+        <v>3.002505</v>
       </c>
       <c r="O32" s="45" t="n">
-        <v>-23.11307007894737</v>
+        <v>1.865544868003026</v>
       </c>
       <c r="P32" s="92" t="n">
-        <v>11.36</v>
+        <v>8.590999999999999</v>
       </c>
       <c r="Q32" s="91" t="n"/>
       <c r="R32" s="33" t="n"/>
@@ -5604,39 +5603,39 @@
       <c r="D33" s="91" t="n"/>
       <c r="E33" s="90" t="inlineStr">
         <is>
-          <t>E2-7</t>
+          <t>E2-1</t>
         </is>
       </c>
       <c r="F33" s="91" t="n"/>
       <c r="G33" s="44" t="n">
-        <v>1.030478</v>
+        <v>-12.032555</v>
       </c>
       <c r="H33" s="42" t="n">
-        <v>1.939033</v>
+        <v>-10.703837</v>
       </c>
       <c r="I33" s="45" t="n">
-        <v>1.469475353204173</v>
+        <v>-11.42275332299013</v>
       </c>
       <c r="J33" s="44" t="n">
-        <v>1.030478</v>
+        <v>-12.032555</v>
       </c>
       <c r="K33" s="42" t="n">
-        <v>2.723479</v>
+        <v>-10.584183</v>
       </c>
       <c r="L33" s="45" t="n">
-        <v>1.765403665041783</v>
+        <v>-11.34177171350984</v>
       </c>
       <c r="M33" s="44" t="n">
-        <v>1.030478</v>
+        <v>-13.143645</v>
       </c>
       <c r="N33" s="42" t="n">
-        <v>3.002505</v>
+        <v>3804.532905</v>
       </c>
       <c r="O33" s="45" t="n">
-        <v>2.061886108108108</v>
+        <v>153.5538822732723</v>
       </c>
       <c r="P33" s="92" t="n">
-        <v>8.590999999999999</v>
+        <v>1.579</v>
       </c>
       <c r="Q33" s="91" t="n"/>
       <c r="R33" s="33" t="n"/>
@@ -5656,39 +5655,39 @@
       <c r="D34" s="91" t="n"/>
       <c r="E34" s="90" t="inlineStr">
         <is>
-          <t>E2-1</t>
+          <t>E2-2</t>
         </is>
       </c>
       <c r="F34" s="91" t="n"/>
       <c r="G34" s="44" t="n">
-        <v>-11.863767</v>
+        <v>-12.622012</v>
       </c>
       <c r="H34" s="42" t="n">
-        <v>-10.584183</v>
+        <v>-10.165668</v>
       </c>
       <c r="I34" s="45" t="n">
-        <v>-11.21115687593423</v>
+        <v>-11.42703736005626</v>
       </c>
       <c r="J34" s="44" t="n">
-        <v>-11.863767</v>
+        <v>-12.622012</v>
       </c>
       <c r="K34" s="42" t="n">
-        <v>-10.446104</v>
+        <v>-10.069366</v>
       </c>
       <c r="L34" s="45" t="n">
-        <v>-11.21664859455687</v>
+        <v>-11.13678622862958</v>
       </c>
       <c r="M34" s="44" t="n">
-        <v>-13.143645</v>
+        <v>-10972.316588</v>
       </c>
       <c r="N34" s="42" t="n">
-        <v>3804.532899</v>
+        <v>3901.509646</v>
       </c>
       <c r="O34" s="45" t="n">
-        <v>139.5010062684853</v>
+        <v>641.7625948581675</v>
       </c>
       <c r="P34" s="92" t="n">
-        <v>1.579</v>
+        <v>1.363</v>
       </c>
       <c r="Q34" s="91" t="n"/>
       <c r="R34" s="33" t="n"/>
@@ -5708,39 +5707,39 @@
       <c r="D35" s="91" t="n"/>
       <c r="E35" s="90" t="inlineStr">
         <is>
-          <t>E2-2</t>
+          <t>E2-5</t>
         </is>
       </c>
       <c r="F35" s="91" t="n"/>
       <c r="G35" s="44" t="n">
-        <v>-11.632942</v>
+        <v>26.844977</v>
       </c>
       <c r="H35" s="42" t="n">
-        <v>-10.069366</v>
+        <v>31.485334</v>
       </c>
       <c r="I35" s="45" t="n">
-        <v>-10.74923281315396</v>
+        <v>29.19328322077922</v>
       </c>
       <c r="J35" s="44" t="n">
-        <v>-11.632942</v>
+        <v>26.820827</v>
       </c>
       <c r="K35" s="42" t="n">
-        <v>-10.069366</v>
+        <v>31.858784</v>
       </c>
       <c r="L35" s="45" t="n">
-        <v>-10.81312715325402</v>
+        <v>29.63570933742331</v>
       </c>
       <c r="M35" s="44" t="n">
-        <v>-8039.385488</v>
+        <v>-0.616</v>
       </c>
       <c r="N35" s="42" t="n">
-        <v>3901.509638</v>
+        <v>35.756319</v>
       </c>
       <c r="O35" s="45" t="n">
-        <v>568.5796442007548</v>
+        <v>30.09807666914498</v>
       </c>
       <c r="P35" s="92" t="n">
-        <v>1.363</v>
+        <v>9.999000000000001</v>
       </c>
       <c r="Q35" s="91" t="n"/>
       <c r="R35" s="33" t="n"/>
@@ -5754,45 +5753,45 @@
       <c r="B36" s="16" t="n"/>
       <c r="C36" s="90" t="inlineStr">
         <is>
-          <t>E1/E2</t>
+          <t>CDIII</t>
         </is>
       </c>
       <c r="D36" s="91" t="n"/>
       <c r="E36" s="90" t="inlineStr">
         <is>
-          <t>E2-5</t>
+          <t>VW-CD3-06</t>
         </is>
       </c>
       <c r="F36" s="91" t="n"/>
       <c r="G36" s="44" t="n">
-        <v>27.405626</v>
+        <v>50.134446</v>
       </c>
       <c r="H36" s="42" t="n">
-        <v>31.858784</v>
+        <v>51.459716</v>
       </c>
       <c r="I36" s="45" t="n">
-        <v>29.8506115974026</v>
+        <v>50.80525436708861</v>
       </c>
       <c r="J36" s="44" t="n">
-        <v>26.820827</v>
+        <v>50.134446</v>
       </c>
       <c r="K36" s="42" t="n">
-        <v>32.396479</v>
+        <v>52.782956</v>
       </c>
       <c r="L36" s="45" t="n">
-        <v>30.10608429012346</v>
+        <v>51.3558303803681</v>
       </c>
       <c r="M36" s="44" t="n">
-        <v>-0.616</v>
+        <v>49.378784</v>
       </c>
       <c r="N36" s="42" t="n">
-        <v>35.756319</v>
+        <v>52.782956</v>
       </c>
       <c r="O36" s="45" t="n">
-        <v>30.33615620089286</v>
+        <v>50.56102996808511</v>
       </c>
       <c r="P36" s="92" t="n">
-        <v>9.999000000000001</v>
+        <v>19.95</v>
       </c>
       <c r="Q36" s="91" t="n"/>
       <c r="R36" s="33" t="n"/>
@@ -5812,39 +5811,39 @@
       <c r="D37" s="91" t="n"/>
       <c r="E37" s="90" t="inlineStr">
         <is>
-          <t>VW-CD3-06</t>
+          <t>VW-CD3-05</t>
         </is>
       </c>
       <c r="F37" s="91" t="n"/>
       <c r="G37" s="44" t="n">
-        <v>51.080402</v>
+        <v>86.635081</v>
       </c>
       <c r="H37" s="42" t="n">
-        <v>52.782956</v>
+        <v>87.39062699999999</v>
       </c>
       <c r="I37" s="45" t="n">
-        <v>51.67980081944444</v>
+        <v>87.04281273863636</v>
       </c>
       <c r="J37" s="44" t="n">
-        <v>49.567697</v>
+        <v>86.635081</v>
       </c>
       <c r="K37" s="42" t="n">
-        <v>52.782956</v>
+        <v>87.957145</v>
       </c>
       <c r="L37" s="45" t="n">
-        <v>51.37679176623377</v>
+        <v>87.18185699999999</v>
       </c>
       <c r="M37" s="44" t="n">
-        <v>49.378784</v>
+        <v>86.067937</v>
       </c>
       <c r="N37" s="42" t="n">
-        <v>52.782956</v>
+        <v>87.957145</v>
       </c>
       <c r="O37" s="45" t="n">
-        <v>50.56908820652174</v>
+        <v>86.86584936312849</v>
       </c>
       <c r="P37" s="92" t="n">
-        <v>19.95</v>
+        <v>27.01599</v>
       </c>
       <c r="Q37" s="91" t="n"/>
       <c r="R37" s="33" t="n"/>
@@ -5863,39 +5862,39 @@
       <c r="D38" s="91" t="n"/>
       <c r="E38" s="90" t="inlineStr">
         <is>
-          <t>VW-CD3-05</t>
+          <t>VW-CD3-02</t>
         </is>
       </c>
       <c r="F38" s="91" t="n"/>
       <c r="G38" s="44" t="n">
-        <v>87.201032</v>
+        <v>52.853332</v>
       </c>
       <c r="H38" s="42" t="n">
-        <v>87.957145</v>
+        <v>53.811959</v>
       </c>
       <c r="I38" s="45" t="n">
-        <v>87.42732379268293</v>
+        <v>53.49361331168831</v>
       </c>
       <c r="J38" s="44" t="n">
-        <v>86.256682</v>
+        <v>52.853273</v>
       </c>
       <c r="K38" s="42" t="n">
-        <v>87.957145</v>
+        <v>53.811959</v>
       </c>
       <c r="L38" s="45" t="n">
-        <v>87.1151893220339</v>
+        <v>53.39935307643312</v>
       </c>
       <c r="M38" s="44" t="n">
-        <v>86.067937</v>
+        <v>52.853229</v>
       </c>
       <c r="N38" s="42" t="n">
-        <v>87.957145</v>
+        <v>54.003621</v>
       </c>
       <c r="O38" s="45" t="n">
-        <v>86.88497886148008</v>
+        <v>53.31385764794816</v>
       </c>
       <c r="P38" s="92" t="n">
-        <v>27.01599</v>
+        <v>69.21399</v>
       </c>
       <c r="Q38" s="91" t="n"/>
       <c r="R38" s="33" t="n"/>
@@ -5908,45 +5907,45 @@
       <c r="B39" s="16" t="n"/>
       <c r="C39" s="90" t="inlineStr">
         <is>
-          <t>CDIII</t>
+          <t>SILT-TRAP</t>
         </is>
       </c>
       <c r="D39" s="91" t="n"/>
       <c r="E39" s="90" t="inlineStr">
         <is>
-          <t>VW-CD3-02</t>
+          <t>VW-ST-06</t>
         </is>
       </c>
       <c r="F39" s="91" t="n"/>
       <c r="G39" s="44" t="n">
-        <v>53.235927</v>
+        <v>89.193048</v>
       </c>
       <c r="H39" s="42" t="n">
-        <v>53.811959</v>
+        <v>90.089845</v>
       </c>
       <c r="I39" s="45" t="n">
-        <v>53.4681854520548</v>
+        <v>89.67193810389611</v>
       </c>
       <c r="J39" s="44" t="n">
-        <v>52.853229</v>
+        <v>87.397784</v>
       </c>
       <c r="K39" s="42" t="n">
-        <v>53.811959</v>
+        <v>90.089845</v>
       </c>
       <c r="L39" s="45" t="n">
-        <v>53.30833427333334</v>
+        <v>88.89550913939394</v>
       </c>
       <c r="M39" s="44" t="n">
-        <v>52.853229</v>
+        <v>87.397784</v>
       </c>
       <c r="N39" s="42" t="n">
-        <v>54.196852</v>
+        <v>90.089845</v>
       </c>
       <c r="O39" s="45" t="n">
-        <v>53.3421802945055</v>
+        <v>88.17319942299349</v>
       </c>
       <c r="P39" s="92" t="n">
-        <v>69.21399</v>
+        <v>14.35099</v>
       </c>
       <c r="Q39" s="91" t="n"/>
       <c r="R39" s="33" t="n"/>
@@ -5958,45 +5957,45 @@
       <c r="B40" s="16" t="n"/>
       <c r="C40" s="90" t="inlineStr">
         <is>
-          <t>SILT-TRAP</t>
+          <t>CDIII</t>
         </is>
       </c>
       <c r="D40" s="91" t="n"/>
       <c r="E40" s="90" t="inlineStr">
         <is>
-          <t>VW-ST-06</t>
+          <t>VW-5</t>
         </is>
       </c>
       <c r="F40" s="91" t="n"/>
       <c r="G40" s="44" t="n">
-        <v>87.397784</v>
+        <v>-8.817121</v>
       </c>
       <c r="H40" s="42" t="n">
-        <v>90.089845</v>
+        <v>-8.28966</v>
       </c>
       <c r="I40" s="45" t="n">
-        <v>88.93646225333333</v>
+        <v>-8.545213626666667</v>
       </c>
       <c r="J40" s="44" t="n">
-        <v>87.397784</v>
+        <v>-8.817121</v>
       </c>
       <c r="K40" s="42" t="n">
-        <v>90.089845</v>
+        <v>-8.114122999999999</v>
       </c>
       <c r="L40" s="45" t="n">
-        <v>88.41186762264151</v>
+        <v>-8.441484857142857</v>
       </c>
       <c r="M40" s="44" t="n">
-        <v>87.397784</v>
+        <v>-8.817121</v>
       </c>
       <c r="N40" s="42" t="n">
-        <v>90.089845</v>
+        <v>-7.674569</v>
       </c>
       <c r="O40" s="45" t="n">
-        <v>87.98482571902655</v>
+        <v>-8.138524926991151</v>
       </c>
       <c r="P40" s="92" t="n">
-        <v>14.35099</v>
+        <v>27.88999</v>
       </c>
       <c r="Q40" s="91" t="n"/>
       <c r="R40" s="33" t="n"/>
@@ -6017,39 +6016,39 @@
       <c r="D41" s="91" t="n"/>
       <c r="E41" s="90" t="inlineStr">
         <is>
-          <t>VW-5</t>
+          <t>VW-4</t>
         </is>
       </c>
       <c r="F41" s="91" t="n"/>
       <c r="G41" s="44" t="n">
-        <v>-8.553742</v>
+        <v>-20.781597</v>
       </c>
       <c r="H41" s="42" t="n">
-        <v>-8.289649000000001</v>
+        <v>-19.912879</v>
       </c>
       <c r="I41" s="45" t="n">
-        <v>-8.389161653333334</v>
+        <v>-20.39123113333333</v>
       </c>
       <c r="J41" s="44" t="n">
-        <v>-8.553742</v>
+        <v>-20.781597</v>
       </c>
       <c r="K41" s="42" t="n">
-        <v>-8.02561</v>
+        <v>-19.719432</v>
       </c>
       <c r="L41" s="45" t="n">
-        <v>-8.305824592105264</v>
+        <v>-20.32498672077922</v>
       </c>
       <c r="M41" s="44" t="n">
-        <v>-8.553742</v>
+        <v>-20.781597</v>
       </c>
       <c r="N41" s="42" t="n">
-        <v>-7.586081</v>
+        <v>-19.719429</v>
       </c>
       <c r="O41" s="45" t="n">
-        <v>-8.050010319101123</v>
+        <v>-20.31471360840708</v>
       </c>
       <c r="P41" s="92" t="n">
-        <v>27.88999</v>
+        <v>25.51999</v>
       </c>
       <c r="Q41" s="91" t="n"/>
       <c r="R41" s="33" t="n"/>
@@ -6070,39 +6069,39 @@
       <c r="D42" s="91" t="n"/>
       <c r="E42" s="90" t="inlineStr">
         <is>
-          <t>VW-4</t>
+          <t>VW-3</t>
         </is>
       </c>
       <c r="F42" s="91" t="n"/>
       <c r="G42" s="44" t="n">
-        <v>-20.588069</v>
+        <v>-22.505086</v>
       </c>
       <c r="H42" s="42" t="n">
-        <v>-19.719432</v>
+        <v>-21.615921</v>
       </c>
       <c r="I42" s="45" t="n">
-        <v>-20.20344696</v>
+        <v>-22.06169776</v>
       </c>
       <c r="J42" s="44" t="n">
-        <v>-20.588069</v>
+        <v>-22.505086</v>
       </c>
       <c r="K42" s="42" t="n">
-        <v>-19.719429</v>
+        <v>-21.349696</v>
       </c>
       <c r="L42" s="45" t="n">
-        <v>-20.21426374342105</v>
+        <v>-21.98201087662338</v>
       </c>
       <c r="M42" s="44" t="n">
-        <v>-20.818728</v>
+        <v>-22.505086</v>
       </c>
       <c r="N42" s="42" t="n">
-        <v>-19.719429</v>
+        <v>-21.349696</v>
       </c>
       <c r="O42" s="45" t="n">
-        <v>-20.31500972134831</v>
+        <v>-21.96490660619469</v>
       </c>
       <c r="P42" s="92" t="n">
-        <v>25.51999</v>
+        <v>23.08999</v>
       </c>
       <c r="Q42" s="91" t="n"/>
       <c r="R42" s="33" t="n"/>
@@ -6123,39 +6122,39 @@
       <c r="D43" s="91" t="n"/>
       <c r="E43" s="90" t="inlineStr">
         <is>
-          <t>VW-3</t>
+          <t>VW-CD3-03</t>
         </is>
       </c>
       <c r="F43" s="91" t="n"/>
       <c r="G43" s="44" t="n">
-        <v>-22.327516</v>
+        <v>45.040171</v>
       </c>
       <c r="H43" s="42" t="n">
-        <v>-21.349696</v>
+        <v>46.194158</v>
       </c>
       <c r="I43" s="45" t="n">
-        <v>-21.8625096</v>
+        <v>45.5579577051282</v>
       </c>
       <c r="J43" s="44" t="n">
-        <v>-22.327516</v>
+        <v>45.040171</v>
       </c>
       <c r="K43" s="42" t="n">
-        <v>-21.349696</v>
+        <v>46.194568</v>
       </c>
       <c r="L43" s="45" t="n">
-        <v>-21.86805617763158</v>
+        <v>45.75129769655172</v>
       </c>
       <c r="M43" s="44" t="n">
-        <v>-22.365794</v>
+        <v>45.040171</v>
       </c>
       <c r="N43" s="42" t="n">
-        <v>-21.349696</v>
+        <v>46.194645</v>
       </c>
       <c r="O43" s="45" t="n">
-        <v>-21.96141191460674</v>
+        <v>45.75398134872979</v>
       </c>
       <c r="P43" s="92" t="n">
-        <v>23.08999</v>
+        <v>30.763</v>
       </c>
       <c r="Q43" s="91" t="n"/>
       <c r="R43" s="33" t="n"/>
@@ -6174,39 +6173,39 @@
       <c r="D44" s="91" t="n"/>
       <c r="E44" s="90" t="inlineStr">
         <is>
-          <t>VW-CD3-03</t>
+          <t>VW-CD3-01</t>
         </is>
       </c>
       <c r="F44" s="91" t="n"/>
       <c r="G44" s="44" t="n">
-        <v>45.424505</v>
+        <v>-0.246418</v>
       </c>
       <c r="H44" s="42" t="n">
-        <v>46.19437</v>
+        <v>0.321405</v>
       </c>
       <c r="I44" s="45" t="n">
-        <v>45.85349086363637</v>
+        <v>0.04895274025974026</v>
       </c>
       <c r="J44" s="44" t="n">
-        <v>45.424505</v>
+        <v>-0.246418</v>
       </c>
       <c r="K44" s="42" t="n">
-        <v>46.194645</v>
+        <v>0.699168</v>
       </c>
       <c r="L44" s="45" t="n">
-        <v>45.88317213669065</v>
+        <v>0.205279050955414</v>
       </c>
       <c r="M44" s="44" t="n">
-        <v>45.424404</v>
+        <v>-0.246418</v>
       </c>
       <c r="N44" s="42" t="n">
-        <v>46.194851</v>
+        <v>1.829548</v>
       </c>
       <c r="O44" s="45" t="n">
-        <v>45.79846712289157</v>
+        <v>0.7764159913606912</v>
       </c>
       <c r="P44" s="92" t="n">
-        <v>30.763</v>
+        <v>51.21899</v>
       </c>
       <c r="Q44" s="91" t="n"/>
       <c r="R44" s="33" t="n"/>
@@ -6225,39 +6224,39 @@
       <c r="D45" s="91" t="n"/>
       <c r="E45" s="90" t="inlineStr">
         <is>
-          <t>VW-CD3-01</t>
+          <t>VW-6</t>
         </is>
       </c>
       <c r="F45" s="91" t="n"/>
       <c r="G45" s="44" t="n">
-        <v>-0.056584</v>
+        <v>-19.846497</v>
       </c>
       <c r="H45" s="42" t="n">
-        <v>0.508927</v>
+        <v>-18.994455</v>
       </c>
       <c r="I45" s="45" t="n">
-        <v>0.2274893698630137</v>
+        <v>-19.43621084615384</v>
       </c>
       <c r="J45" s="44" t="n">
-        <v>-0.056584</v>
+        <v>-19.846497</v>
       </c>
       <c r="K45" s="42" t="n">
-        <v>0.887259</v>
+        <v>-18.804534</v>
       </c>
       <c r="L45" s="45" t="n">
-        <v>0.3821992266666667</v>
+        <v>-19.35568364705883</v>
       </c>
       <c r="M45" s="44" t="n">
-        <v>-0.056584</v>
+        <v>-19.846497</v>
       </c>
       <c r="N45" s="42" t="n">
-        <v>2.338828</v>
+        <v>-18.804534</v>
       </c>
       <c r="O45" s="45" t="n">
-        <v>1.009730635164835</v>
+        <v>-19.33583890343348</v>
       </c>
       <c r="P45" s="92" t="n">
-        <v>51.21899</v>
+        <v>23.14199</v>
       </c>
       <c r="Q45" s="91" t="n"/>
       <c r="R45" s="33" t="n"/>
@@ -6276,39 +6275,39 @@
       <c r="D46" s="91" t="n"/>
       <c r="E46" s="90" t="inlineStr">
         <is>
-          <t>VW-6</t>
+          <t>VW-7</t>
         </is>
       </c>
       <c r="F46" s="91" t="n"/>
       <c r="G46" s="44" t="n">
-        <v>-19.751891</v>
+        <v>-19.021025</v>
       </c>
       <c r="H46" s="42" t="n">
-        <v>-18.804534</v>
+        <v>-18.27188</v>
       </c>
       <c r="I46" s="45" t="n">
-        <v>-19.22448962162162</v>
+        <v>-18.60796235897436</v>
       </c>
       <c r="J46" s="44" t="n">
-        <v>-19.751891</v>
+        <v>-19.021025</v>
       </c>
       <c r="K46" s="42" t="n">
-        <v>-18.804534</v>
+        <v>-18.084062</v>
       </c>
       <c r="L46" s="45" t="n">
-        <v>-19.24733796598639</v>
+        <v>-18.53918762745098</v>
       </c>
       <c r="M46" s="44" t="n">
-        <v>-19.916199</v>
+        <v>-19.021025</v>
       </c>
       <c r="N46" s="42" t="n">
-        <v>-18.804534</v>
+        <v>-18.084058</v>
       </c>
       <c r="O46" s="45" t="n">
-        <v>-19.36064628227571</v>
+        <v>-18.52711287982833</v>
       </c>
       <c r="P46" s="92" t="n">
-        <v>23.14199</v>
+        <v>25.399</v>
       </c>
       <c r="Q46" s="91" t="n"/>
       <c r="R46" s="33" t="n"/>
@@ -6327,39 +6326,39 @@
       <c r="D47" s="91" t="n"/>
       <c r="E47" s="90" t="inlineStr">
         <is>
-          <t>VW-7</t>
+          <t>VW-8</t>
         </is>
       </c>
       <c r="F47" s="91" t="n"/>
       <c r="G47" s="44" t="n">
-        <v>-18.833903</v>
+        <v>-21.426288</v>
       </c>
       <c r="H47" s="42" t="n">
-        <v>-18.084062</v>
+        <v>-20.618181</v>
       </c>
       <c r="I47" s="45" t="n">
-        <v>-18.41972856756757</v>
+        <v>-21.04406637179487</v>
       </c>
       <c r="J47" s="44" t="n">
-        <v>-18.833903</v>
+        <v>-21.426288</v>
       </c>
       <c r="K47" s="42" t="n">
-        <v>-18.084058</v>
+        <v>-20.348639</v>
       </c>
       <c r="L47" s="45" t="n">
-        <v>-18.43219091836735</v>
+        <v>-20.97084981045752</v>
       </c>
       <c r="M47" s="44" t="n">
-        <v>-19.005903</v>
+        <v>-21.515917</v>
       </c>
       <c r="N47" s="42" t="n">
-        <v>-18.084058</v>
+        <v>-20.348639</v>
       </c>
       <c r="O47" s="45" t="n">
-        <v>-18.53324473960613</v>
+        <v>-20.95974259227468</v>
       </c>
       <c r="P47" s="92" t="n">
-        <v>25.399</v>
+        <v>28.498</v>
       </c>
       <c r="Q47" s="91" t="n"/>
       <c r="R47" s="33" t="n"/>
@@ -6378,39 +6377,39 @@
       <c r="D48" s="91" t="n"/>
       <c r="E48" s="90" t="inlineStr">
         <is>
-          <t>VW-8</t>
+          <t>VW-9</t>
         </is>
       </c>
       <c r="F48" s="91" t="n"/>
       <c r="G48" s="44" t="n">
-        <v>-21.247004</v>
+        <v>-11.386236</v>
       </c>
       <c r="H48" s="42" t="n">
-        <v>-20.348639</v>
+        <v>-10.462811</v>
       </c>
       <c r="I48" s="45" t="n">
-        <v>-20.8377695</v>
+        <v>-10.89517815384615</v>
       </c>
       <c r="J48" s="44" t="n">
-        <v>-21.247004</v>
+        <v>-11.386236</v>
       </c>
       <c r="K48" s="42" t="n">
-        <v>-20.348639</v>
+        <v>-10.186349</v>
       </c>
       <c r="L48" s="45" t="n">
-        <v>-20.85880034693878</v>
+        <v>-10.77082309803922</v>
       </c>
       <c r="M48" s="44" t="n">
-        <v>-21.660878</v>
+        <v>-11.386236</v>
       </c>
       <c r="N48" s="42" t="n">
-        <v>-20.348639</v>
+        <v>-9.816964</v>
       </c>
       <c r="O48" s="45" t="n">
-        <v>-20.98222527789934</v>
+        <v>-10.42974128540773</v>
       </c>
       <c r="P48" s="92" t="n">
-        <v>28.498</v>
+        <v>29.74</v>
       </c>
       <c r="Q48" s="91" t="n"/>
       <c r="R48" s="33" t="n"/>
@@ -6423,45 +6422,45 @@
       <c r="B49" s="16" t="n"/>
       <c r="C49" s="90" t="inlineStr">
         <is>
-          <t>CDIII</t>
+          <t>SILT-TRAP</t>
         </is>
       </c>
       <c r="D49" s="91" t="n"/>
       <c r="E49" s="90" t="inlineStr">
         <is>
-          <t>VW-9</t>
+          <t>VW-ST-01</t>
         </is>
       </c>
       <c r="F49" s="91" t="n"/>
       <c r="G49" s="44" t="n">
-        <v>-10.924474</v>
+        <v>37.378567</v>
       </c>
       <c r="H49" s="42" t="n">
-        <v>-10.186349</v>
+        <v>37.948398</v>
       </c>
       <c r="I49" s="45" t="n">
-        <v>-10.67512641891892</v>
+        <v>37.69448046666667</v>
       </c>
       <c r="J49" s="44" t="n">
-        <v>-10.924474</v>
+        <v>36.999727</v>
       </c>
       <c r="K49" s="42" t="n">
-        <v>-10.186332</v>
+        <v>37.948398</v>
       </c>
       <c r="L49" s="45" t="n">
-        <v>-10.6125063877551</v>
+        <v>37.45757047651006</v>
       </c>
       <c r="M49" s="44" t="n">
-        <v>-10.924474</v>
+        <v>36.999727</v>
       </c>
       <c r="N49" s="42" t="n">
-        <v>-9.801826</v>
+        <v>37.948398</v>
       </c>
       <c r="O49" s="45" t="n">
-        <v>-10.35696403063457</v>
+        <v>37.38289700217391</v>
       </c>
       <c r="P49" s="92" t="n">
-        <v>29.74</v>
+        <v>42.52999</v>
       </c>
       <c r="Q49" s="91" t="n"/>
       <c r="R49" s="1" t="n"/>
@@ -6474,45 +6473,45 @@
       <c r="B50" s="16" t="n"/>
       <c r="C50" s="90" t="inlineStr">
         <is>
-          <t>SILT-TRAP</t>
+          <t>CROWN</t>
         </is>
       </c>
       <c r="D50" s="91" t="n"/>
       <c r="E50" s="90" t="inlineStr">
         <is>
-          <t>VW-ST-01</t>
+          <t>VW-44</t>
         </is>
       </c>
       <c r="F50" s="91" t="n"/>
       <c r="G50" s="44" t="n">
-        <v>36.999727</v>
+        <v>-21.95987</v>
       </c>
       <c r="H50" s="42" t="n">
-        <v>37.757572</v>
+        <v>-21.211033</v>
       </c>
       <c r="I50" s="45" t="n">
-        <v>37.3758615882353</v>
+        <v>-21.59020633688699</v>
       </c>
       <c r="J50" s="44" t="n">
-        <v>36.999727</v>
+        <v>-21.95987</v>
       </c>
       <c r="K50" s="42" t="n">
-        <v>37.757572</v>
+        <v>-20.930106</v>
       </c>
       <c r="L50" s="45" t="n">
-        <v>37.28919504794521</v>
+        <v>-21.51814880656186</v>
       </c>
       <c r="M50" s="44" t="n">
-        <v>36.999727</v>
+        <v>-21.95987</v>
       </c>
       <c r="N50" s="42" t="n">
-        <v>37.757572</v>
+        <v>-20.930104</v>
       </c>
       <c r="O50" s="45" t="n">
-        <v>37.34539672787611</v>
+        <v>-21.50097865879479</v>
       </c>
       <c r="P50" s="92" t="n">
-        <v>42.52999</v>
+        <v>26.038</v>
       </c>
       <c r="Q50" s="91" t="n"/>
       <c r="R50" s="1" t="n"/>
@@ -6525,45 +6524,45 @@
       <c r="B51" s="16" t="n"/>
       <c r="C51" s="90" t="inlineStr">
         <is>
-          <t>SILT-TRAP</t>
+          <t>CROWN</t>
         </is>
       </c>
       <c r="D51" s="91" t="n"/>
       <c r="E51" s="90" t="inlineStr">
         <is>
-          <t>VW-ST-02</t>
+          <t>VW-CN-02</t>
         </is>
       </c>
       <c r="F51" s="91" t="n"/>
       <c r="G51" s="44" t="n">
-        <v>30.702714</v>
+        <v>-8.846880000000001</v>
       </c>
       <c r="H51" s="42" t="n">
-        <v>32.441615</v>
+        <v>-5.213875</v>
       </c>
       <c r="I51" s="45" t="n">
-        <v>31.5481805</v>
+        <v>-7.275529342465753</v>
       </c>
       <c r="J51" s="44" t="n">
-        <v>30.702714</v>
+        <v>-9.230142000000001</v>
       </c>
       <c r="K51" s="42" t="n">
-        <v>32.441615</v>
+        <v>-5.213786</v>
       </c>
       <c r="L51" s="45" t="n">
-        <v>31.29521175193798</v>
+        <v>-7.159668660130719</v>
       </c>
       <c r="M51" s="44" t="n">
-        <v>30.70271</v>
+        <v>-9.802917000000001</v>
       </c>
       <c r="N51" s="42" t="n">
-        <v>32.441615</v>
+        <v>-5.213486</v>
       </c>
       <c r="O51" s="45" t="n">
-        <v>31.1543193187067</v>
+        <v>-7.219232283549784</v>
       </c>
       <c r="P51" s="92" t="n">
-        <v>18.40499</v>
+        <v>39.7</v>
       </c>
       <c r="Q51" s="91" t="n"/>
       <c r="R51" s="1" t="n"/>
@@ -6576,45 +6575,45 @@
       <c r="B52" s="16" t="n"/>
       <c r="C52" s="90" t="inlineStr">
         <is>
-          <t>CROWN</t>
+          <t>SILT-TRAP</t>
         </is>
       </c>
       <c r="D52" s="91" t="n"/>
       <c r="E52" s="90" t="inlineStr">
         <is>
-          <t>VW-44</t>
+          <t>VW-21</t>
         </is>
       </c>
       <c r="F52" s="91" t="n"/>
       <c r="G52" s="44" t="n">
-        <v>-21.865663</v>
+        <v>-417.943342</v>
       </c>
       <c r="H52" s="42" t="n">
-        <v>-20.930106</v>
+        <v>-417.407769</v>
       </c>
       <c r="I52" s="45" t="n">
-        <v>-21.40572280210685</v>
+        <v>-417.6774924578313</v>
       </c>
       <c r="J52" s="44" t="n">
-        <v>-21.865663</v>
+        <v>-417.943342</v>
       </c>
       <c r="K52" s="42" t="n">
-        <v>-20.930104</v>
+        <v>-417.193024</v>
       </c>
       <c r="L52" s="45" t="n">
-        <v>-21.40652048211781</v>
+        <v>-417.5592329602273</v>
       </c>
       <c r="M52" s="44" t="n">
-        <v>-22.029527</v>
+        <v>-417.943342</v>
       </c>
       <c r="N52" s="42" t="n">
-        <v>-20.930104</v>
+        <v>-416.657597</v>
       </c>
       <c r="O52" s="45" t="n">
-        <v>-21.50695356904113</v>
+        <v>-417.2892113007812</v>
       </c>
       <c r="P52" s="92" t="n">
-        <v>26.038</v>
+        <v>16.262</v>
       </c>
       <c r="Q52" s="91" t="n"/>
       <c r="R52" s="1" t="n"/>
@@ -6626,45 +6625,45 @@
       <c r="B53" s="16" t="n"/>
       <c r="C53" s="90" t="inlineStr">
         <is>
-          <t>CROWN</t>
+          <t>SILT-TRAP</t>
         </is>
       </c>
       <c r="D53" s="91" t="n"/>
       <c r="E53" s="90" t="inlineStr">
         <is>
-          <t>VW-CN-02</t>
+          <t>VW-22</t>
         </is>
       </c>
       <c r="F53" s="91" t="n"/>
       <c r="G53" s="44" t="n">
-        <v>-8.655887999999999</v>
+        <v>151.617395</v>
       </c>
       <c r="H53" s="42" t="n">
-        <v>-5.213875</v>
+        <v>152.133393</v>
       </c>
       <c r="I53" s="45" t="n">
-        <v>-7.057294585714286</v>
+        <v>151.8335114457831</v>
       </c>
       <c r="J53" s="44" t="n">
-        <v>-9.230392</v>
+        <v>151.617395</v>
       </c>
       <c r="K53" s="42" t="n">
-        <v>-5.213786</v>
+        <v>152.394122</v>
       </c>
       <c r="L53" s="45" t="n">
-        <v>-7.041360914473684</v>
+        <v>151.9446698977273</v>
       </c>
       <c r="M53" s="44" t="n">
-        <v>-9.802917000000001</v>
+        <v>151.617395</v>
       </c>
       <c r="N53" s="42" t="n">
-        <v>-5.213486</v>
+        <v>152.652854</v>
       </c>
       <c r="O53" s="45" t="n">
-        <v>-7.196179515555555</v>
+        <v>152.2086747324219</v>
       </c>
       <c r="P53" s="92" t="n">
-        <v>39.7</v>
+        <v>22.271</v>
       </c>
       <c r="Q53" s="91" t="n"/>
       <c r="R53" s="1" t="n"/>
@@ -6682,39 +6681,39 @@
       <c r="D54" s="91" t="n"/>
       <c r="E54" s="90" t="inlineStr">
         <is>
-          <t>VW-21</t>
+          <t>VW-23</t>
         </is>
       </c>
       <c r="F54" s="91" t="n"/>
       <c r="G54" s="44" t="n">
-        <v>-417.729444</v>
+        <v>-24.407596</v>
       </c>
       <c r="H54" s="42" t="n">
-        <v>-417.19304</v>
+        <v>-23.606059</v>
       </c>
       <c r="I54" s="45" t="n">
-        <v>-417.5014747283951</v>
+        <v>-24.02718489156626</v>
       </c>
       <c r="J54" s="44" t="n">
-        <v>-417.729444</v>
+        <v>-24.407597</v>
       </c>
       <c r="K54" s="42" t="n">
-        <v>-416.872295</v>
+        <v>-23.406138</v>
       </c>
       <c r="L54" s="45" t="n">
-        <v>-417.3820920813953</v>
+        <v>-23.99930540909091</v>
       </c>
       <c r="M54" s="44" t="n">
-        <v>-417.729444</v>
+        <v>-24.908504</v>
       </c>
       <c r="N54" s="42" t="n">
-        <v>-416.657597</v>
+        <v>-23.406138</v>
       </c>
       <c r="O54" s="45" t="n">
-        <v>-417.1886839780876</v>
+        <v>-24.1843818203125</v>
       </c>
       <c r="P54" s="92" t="n">
-        <v>16.262</v>
+        <v>2.21599</v>
       </c>
       <c r="Q54" s="91" t="n"/>
       <c r="R54" s="1" t="n"/>
@@ -6732,39 +6731,39 @@
       <c r="D55" s="91" t="n"/>
       <c r="E55" s="90" t="inlineStr">
         <is>
-          <t>VW-22</t>
+          <t>VW-24</t>
         </is>
       </c>
       <c r="F55" s="91" t="n"/>
       <c r="G55" s="44" t="n">
-        <v>151.74902</v>
+        <v>-23.185277</v>
       </c>
       <c r="H55" s="42" t="n">
-        <v>152.265912</v>
+        <v>-22.36433</v>
       </c>
       <c r="I55" s="45" t="n">
-        <v>151.969542037037</v>
+        <v>-22.84151509638554</v>
       </c>
       <c r="J55" s="44" t="n">
-        <v>151.74902</v>
+        <v>-23.185277</v>
       </c>
       <c r="K55" s="42" t="n">
-        <v>152.523885</v>
+        <v>-22.182279</v>
       </c>
       <c r="L55" s="45" t="n">
-        <v>152.1084265523256</v>
+        <v>-22.75997754545455</v>
       </c>
       <c r="M55" s="44" t="n">
-        <v>151.74902</v>
+        <v>-23.185277</v>
       </c>
       <c r="N55" s="42" t="n">
-        <v>152.652854</v>
+        <v>-22.182279</v>
       </c>
       <c r="O55" s="45" t="n">
-        <v>152.2862369342629</v>
+        <v>-22.7363411796875</v>
       </c>
       <c r="P55" s="92" t="n">
-        <v>22.271</v>
+        <v>7.395</v>
       </c>
       <c r="Q55" s="91" t="n"/>
       <c r="R55" s="1" t="n"/>
@@ -6776,45 +6775,45 @@
       <c r="B56" s="16" t="n"/>
       <c r="C56" s="90" t="inlineStr">
         <is>
-          <t>SILT-TRAP</t>
+          <t>RDS</t>
         </is>
       </c>
       <c r="D56" s="91" t="n"/>
       <c r="E56" s="90" t="inlineStr">
         <is>
-          <t>VW-23</t>
+          <t>VW-RDS-02</t>
         </is>
       </c>
       <c r="F56" s="91" t="n"/>
       <c r="G56" s="44" t="n">
-        <v>-24.407597</v>
+        <v>41.524902</v>
       </c>
       <c r="H56" s="42" t="n">
-        <v>-23.406138</v>
+        <v>43.894174</v>
       </c>
       <c r="I56" s="45" t="n">
-        <v>-23.88180428395062</v>
+        <v>43.00893394666667</v>
       </c>
       <c r="J56" s="44" t="n">
-        <v>-24.4076</v>
+        <v>41.524902</v>
       </c>
       <c r="K56" s="42" t="n">
-        <v>-23.406138</v>
+        <v>43.894174</v>
       </c>
       <c r="L56" s="45" t="n">
-        <v>-23.9449855872093</v>
+        <v>42.88650601282051</v>
       </c>
       <c r="M56" s="44" t="n">
-        <v>-25.025926</v>
+        <v>40.977668</v>
       </c>
       <c r="N56" s="42" t="n">
-        <v>-23.406138</v>
+        <v>44.258144</v>
       </c>
       <c r="O56" s="45" t="n">
-        <v>-24.24576913545817</v>
+        <v>42.72158206170213</v>
       </c>
       <c r="P56" s="92" t="n">
-        <v>2.21599</v>
+        <v>44.82999</v>
       </c>
       <c r="Q56" s="91" t="n"/>
       <c r="R56" s="1" t="n"/>
@@ -6826,45 +6825,45 @@
       <c r="B57" s="16" t="n"/>
       <c r="C57" s="90" t="inlineStr">
         <is>
-          <t>SILT-TRAP</t>
+          <t>RDS</t>
         </is>
       </c>
       <c r="D57" s="91" t="n"/>
       <c r="E57" s="90" t="inlineStr">
         <is>
-          <t>VW-24</t>
+          <t>VW-35</t>
         </is>
       </c>
       <c r="F57" s="91" t="n"/>
       <c r="G57" s="44" t="n">
-        <v>-23.003153</v>
+        <v>-26.42867</v>
       </c>
       <c r="H57" s="42" t="n">
-        <v>-22.182279</v>
+        <v>-20.166987</v>
       </c>
       <c r="I57" s="45" t="n">
-        <v>-22.63932795061728</v>
+        <v>-23.36543305</v>
       </c>
       <c r="J57" s="44" t="n">
-        <v>-23.094213</v>
+        <v>-27.016474</v>
       </c>
       <c r="K57" s="42" t="n">
-        <v>-22.182279</v>
+        <v>-20.166987</v>
       </c>
       <c r="L57" s="45" t="n">
-        <v>-22.65674620930233</v>
+        <v>-23.27148362424242</v>
       </c>
       <c r="M57" s="44" t="n">
-        <v>-23.296956</v>
+        <v>-27.016474</v>
       </c>
       <c r="N57" s="42" t="n">
-        <v>-22.182279</v>
+        <v>-18.79994</v>
       </c>
       <c r="O57" s="45" t="n">
-        <v>-22.74881862350598</v>
+        <v>-23.260602714</v>
       </c>
       <c r="P57" s="92" t="n">
-        <v>7.395</v>
+        <v>21.20299</v>
       </c>
       <c r="Q57" s="91" t="n"/>
       <c r="R57" s="1" t="n"/>
@@ -6882,39 +6881,39 @@
       <c r="D58" s="91" t="n"/>
       <c r="E58" s="90" t="inlineStr">
         <is>
-          <t>VW-RDS-02</t>
+          <t>VW-36</t>
         </is>
       </c>
       <c r="F58" s="91" t="n"/>
       <c r="G58" s="44" t="n">
-        <v>41.524902</v>
+        <v>-27.944264</v>
       </c>
       <c r="H58" s="42" t="n">
-        <v>43.894174</v>
+        <v>-20.267029</v>
       </c>
       <c r="I58" s="45" t="n">
-        <v>42.90451329333333</v>
+        <v>-23.487423275</v>
       </c>
       <c r="J58" s="44" t="n">
-        <v>41.524902</v>
+        <v>-27.944264</v>
       </c>
       <c r="K58" s="42" t="n">
-        <v>43.894174</v>
+        <v>-19.77595</v>
       </c>
       <c r="L58" s="45" t="n">
-        <v>42.81435550649351</v>
+        <v>-23.29964812121212</v>
       </c>
       <c r="M58" s="44" t="n">
-        <v>40.977668</v>
+        <v>-27.944264</v>
       </c>
       <c r="N58" s="42" t="n">
-        <v>44.258144</v>
+        <v>-18.99009</v>
       </c>
       <c r="O58" s="45" t="n">
-        <v>42.71864394396552</v>
+        <v>-23.333202714</v>
       </c>
       <c r="P58" s="92" t="n">
-        <v>44.82999</v>
+        <v>10.273</v>
       </c>
       <c r="Q58" s="91" t="n"/>
       <c r="R58" s="1" t="n"/>
@@ -6926,45 +6925,45 @@
       <c r="B59" s="16" t="n"/>
       <c r="C59" s="90" t="inlineStr">
         <is>
-          <t>RDS</t>
+          <t>CROWN</t>
         </is>
       </c>
       <c r="D59" s="91" t="n"/>
       <c r="E59" s="90" t="inlineStr">
         <is>
-          <t>VW-35</t>
+          <t>VW-49</t>
         </is>
       </c>
       <c r="F59" s="91" t="n"/>
       <c r="G59" s="44" t="n">
-        <v>-26.428672</v>
+        <v>-21.404828</v>
       </c>
       <c r="H59" s="42" t="n">
-        <v>-20.166987</v>
+        <v>-20.818469</v>
       </c>
       <c r="I59" s="45" t="n">
-        <v>-23.25795426666667</v>
+        <v>-21.17104532857143</v>
       </c>
       <c r="J59" s="44" t="n">
-        <v>-27.016474</v>
+        <v>-21.404828</v>
       </c>
       <c r="K59" s="42" t="n">
-        <v>-18.79994</v>
+        <v>-20.678782</v>
       </c>
       <c r="L59" s="45" t="n">
-        <v>-23.19680516149068</v>
+        <v>-21.0884003625</v>
       </c>
       <c r="M59" s="44" t="n">
-        <v>-27.016474</v>
+        <v>-21.456513</v>
       </c>
       <c r="N59" s="42" t="n">
-        <v>-18.79994</v>
+        <v>-20.642441</v>
       </c>
       <c r="O59" s="45" t="n">
-        <v>-23.23285359958932</v>
+        <v>-21.077840794926</v>
       </c>
       <c r="P59" s="92" t="n">
-        <v>21.20299</v>
+        <v>25.036</v>
       </c>
       <c r="Q59" s="91" t="n"/>
       <c r="R59" s="1" t="n"/>
@@ -6976,45 +6975,45 @@
       <c r="B60" s="16" t="n"/>
       <c r="C60" s="90" t="inlineStr">
         <is>
-          <t>RDS</t>
+          <t>CROWN</t>
         </is>
       </c>
       <c r="D60" s="91" t="n"/>
       <c r="E60" s="90" t="inlineStr">
         <is>
-          <t>VW-36</t>
+          <t>VW-48</t>
         </is>
       </c>
       <c r="F60" s="91" t="n"/>
       <c r="G60" s="44" t="n">
-        <v>-27.944264</v>
+        <v>-23.750894</v>
       </c>
       <c r="H60" s="42" t="n">
-        <v>-19.77595</v>
+        <v>-23.071471</v>
       </c>
       <c r="I60" s="45" t="n">
-        <v>-23.22864189333333</v>
+        <v>-23.4490843</v>
       </c>
       <c r="J60" s="44" t="n">
-        <v>-27.944264</v>
+        <v>-23.750894</v>
       </c>
       <c r="K60" s="42" t="n">
-        <v>-18.99009</v>
+        <v>-22.922021</v>
       </c>
       <c r="L60" s="45" t="n">
-        <v>-23.18745045341615</v>
+        <v>-23.36096784375</v>
       </c>
       <c r="M60" s="44" t="n">
-        <v>-27.944264</v>
+        <v>-23.778583</v>
       </c>
       <c r="N60" s="42" t="n">
-        <v>-18.99009</v>
+        <v>-22.922021</v>
       </c>
       <c r="O60" s="45" t="n">
-        <v>-23.31634019917864</v>
+        <v>-23.37444419661734</v>
       </c>
       <c r="P60" s="92" t="n">
-        <v>10.273</v>
+        <v>23.666</v>
       </c>
       <c r="Q60" s="91" t="n"/>
       <c r="R60" s="1" t="n"/>
@@ -7032,39 +7031,39 @@
       <c r="D61" s="91" t="n"/>
       <c r="E61" s="90" t="inlineStr">
         <is>
-          <t>VW-49</t>
+          <t>VW-47</t>
         </is>
       </c>
       <c r="F61" s="91" t="n"/>
       <c r="G61" s="44" t="n">
-        <v>-21.315969</v>
+        <v>-23.611537</v>
       </c>
       <c r="H61" s="42" t="n">
-        <v>-20.678782</v>
+        <v>-22.899291</v>
       </c>
       <c r="I61" s="45" t="n">
-        <v>-20.98366038571428</v>
+        <v>-23.28484005714286</v>
       </c>
       <c r="J61" s="44" t="n">
-        <v>-21.315969</v>
+        <v>-23.611537</v>
       </c>
       <c r="K61" s="42" t="n">
-        <v>-20.642441</v>
+        <v>-22.660502</v>
       </c>
       <c r="L61" s="45" t="n">
-        <v>-20.98647565625</v>
+        <v>-23.18485233125</v>
       </c>
       <c r="M61" s="44" t="n">
-        <v>-21.536199</v>
+        <v>-23.618703</v>
       </c>
       <c r="N61" s="42" t="n">
-        <v>-20.642441</v>
+        <v>-22.660502</v>
       </c>
       <c r="O61" s="45" t="n">
-        <v>-21.08452818736383</v>
+        <v>-23.16515778646934</v>
       </c>
       <c r="P61" s="92" t="n">
-        <v>25.036</v>
+        <v>21.137</v>
       </c>
       <c r="Q61" s="91" t="n"/>
       <c r="R61" s="1" t="n"/>
@@ -7082,39 +7081,39 @@
       <c r="D62" s="91" t="n"/>
       <c r="E62" s="90" t="inlineStr">
         <is>
-          <t>VW-48</t>
+          <t>VW-51</t>
         </is>
       </c>
       <c r="F62" s="91" t="n"/>
       <c r="G62" s="44" t="n">
-        <v>-23.550755</v>
+        <v>10.919547</v>
       </c>
       <c r="H62" s="42" t="n">
-        <v>-22.922021</v>
+        <v>11.359651</v>
       </c>
       <c r="I62" s="45" t="n">
-        <v>-23.26068378571428</v>
+        <v>11.11930733333333</v>
       </c>
       <c r="J62" s="44" t="n">
-        <v>-23.550755</v>
+        <v>10.189202</v>
       </c>
       <c r="K62" s="42" t="n">
-        <v>-22.922021</v>
+        <v>11.359651</v>
       </c>
       <c r="L62" s="45" t="n">
-        <v>-23.2584379375</v>
+        <v>10.91230783139535</v>
       </c>
       <c r="M62" s="44" t="n">
-        <v>-23.952188</v>
+        <v>8.288736999999999</v>
       </c>
       <c r="N62" s="42" t="n">
-        <v>-22.922021</v>
+        <v>11.359651</v>
       </c>
       <c r="O62" s="45" t="n">
-        <v>-23.40466076252723</v>
+        <v>9.817323218436874</v>
       </c>
       <c r="P62" s="92" t="n">
-        <v>23.666</v>
+        <v>30.597</v>
       </c>
       <c r="Q62" s="91" t="n"/>
       <c r="R62" s="1" t="n"/>
@@ -7132,39 +7131,39 @@
       <c r="D63" s="91" t="n"/>
       <c r="E63" s="90" t="inlineStr">
         <is>
-          <t>VW-47</t>
+          <t>VW-50</t>
         </is>
       </c>
       <c r="F63" s="91" t="n"/>
       <c r="G63" s="44" t="n">
-        <v>-23.447972</v>
+        <v>-6.449286</v>
       </c>
       <c r="H63" s="42" t="n">
-        <v>-22.660502</v>
+        <v>-5.623624</v>
       </c>
       <c r="I63" s="45" t="n">
-        <v>-23.06859944285714</v>
+        <v>-6.020674139534884</v>
       </c>
       <c r="J63" s="44" t="n">
-        <v>-23.447972</v>
+        <v>-6.449286</v>
       </c>
       <c r="K63" s="42" t="n">
-        <v>-22.660502</v>
+        <v>-5.486587</v>
       </c>
       <c r="L63" s="45" t="n">
-        <v>-23.07190351875</v>
+        <v>-5.96032801734104</v>
       </c>
       <c r="M63" s="44" t="n">
-        <v>-23.5351</v>
+        <v>-6.595391</v>
       </c>
       <c r="N63" s="42" t="n">
-        <v>-22.660502</v>
+        <v>-5.486587</v>
       </c>
       <c r="O63" s="45" t="n">
-        <v>-23.13251426143791</v>
+        <v>-6.008198926356589</v>
       </c>
       <c r="P63" s="92" t="n">
-        <v>21.137</v>
+        <v>16.459</v>
       </c>
       <c r="Q63" s="91" t="n"/>
       <c r="R63" s="1" t="n"/>
@@ -7176,45 +7175,45 @@
       <c r="B64" s="16" t="n"/>
       <c r="C64" s="90" t="inlineStr">
         <is>
-          <t>CROWN</t>
+          <t>Z1</t>
         </is>
       </c>
       <c r="D64" s="91" t="n"/>
       <c r="E64" s="90" t="inlineStr">
         <is>
-          <t>VW-51</t>
+          <t>VW-ZB-02</t>
         </is>
       </c>
       <c r="F64" s="91" t="n"/>
       <c r="G64" s="44" t="n">
-        <v>10.773243</v>
+        <v>31.055932</v>
       </c>
       <c r="H64" s="42" t="n">
-        <v>11.213607</v>
+        <v>34.825272</v>
       </c>
       <c r="I64" s="45" t="n">
-        <v>10.99386724390244</v>
+        <v>32.87792022972973</v>
       </c>
       <c r="J64" s="44" t="n">
-        <v>9.60493</v>
+        <v>31.055932</v>
       </c>
       <c r="K64" s="42" t="n">
-        <v>11.213607</v>
+        <v>35.015155</v>
       </c>
       <c r="L64" s="45" t="n">
-        <v>10.61301367630058</v>
+        <v>33.29382923684211</v>
       </c>
       <c r="M64" s="44" t="n">
-        <v>8.288736999999999</v>
+        <v>24.075044</v>
       </c>
       <c r="N64" s="42" t="n">
-        <v>11.213607</v>
+        <v>35.015155</v>
       </c>
       <c r="O64" s="45" t="n">
-        <v>9.67093916194332</v>
+        <v>28.64367865726681</v>
       </c>
       <c r="P64" s="92" t="n">
-        <v>30.597</v>
+        <v>14.764</v>
       </c>
       <c r="Q64" s="91" t="n"/>
       <c r="R64" s="1" t="n"/>
@@ -7226,45 +7225,45 @@
       <c r="B65" s="16" t="n"/>
       <c r="C65" s="90" t="inlineStr">
         <is>
-          <t>CROWN</t>
+          <t>Z1</t>
         </is>
       </c>
       <c r="D65" s="91" t="n"/>
       <c r="E65" s="90" t="inlineStr">
         <is>
-          <t>VW-50</t>
+          <t>VW-ZC-01</t>
         </is>
       </c>
       <c r="F65" s="91" t="n"/>
       <c r="G65" s="44" t="n">
-        <v>-6.176628</v>
+        <v>-7.447876</v>
       </c>
       <c r="H65" s="42" t="n">
-        <v>-5.486587</v>
+        <v>-6.526014</v>
       </c>
       <c r="I65" s="45" t="n">
-        <v>-5.842363189873418</v>
+        <v>-6.961482578313253</v>
       </c>
       <c r="J65" s="44" t="n">
-        <v>-6.177636</v>
+        <v>-7.447876</v>
       </c>
       <c r="K65" s="42" t="n">
-        <v>-5.486587</v>
+        <v>-5.972408</v>
       </c>
       <c r="L65" s="45" t="n">
-        <v>-5.868860101190476</v>
+        <v>-6.644348897142857</v>
       </c>
       <c r="M65" s="44" t="n">
-        <v>-6.830049</v>
+        <v>-7.447876</v>
       </c>
       <c r="N65" s="42" t="n">
-        <v>-5.486587</v>
+        <v>-3.390861</v>
       </c>
       <c r="O65" s="45" t="n">
-        <v>-6.06330248</v>
+        <v>-5.501527157088122</v>
       </c>
       <c r="P65" s="92" t="n">
-        <v>16.459</v>
+        <v>8.31</v>
       </c>
       <c r="Q65" s="91" t="n"/>
       <c r="R65" s="1" t="n"/>
@@ -7276,45 +7275,45 @@
       <c r="B66" s="16" t="n"/>
       <c r="C66" s="90" t="inlineStr">
         <is>
-          <t>Z1</t>
+          <t>SILT-TRAP</t>
         </is>
       </c>
       <c r="D66" s="91" t="n"/>
       <c r="E66" s="90" t="inlineStr">
         <is>
-          <t>VW-ZB-02</t>
+          <t>VW-27</t>
         </is>
       </c>
       <c r="F66" s="91" t="n"/>
       <c r="G66" s="44" t="n">
-        <v>33.318871</v>
+        <v>-68.940006</v>
       </c>
       <c r="H66" s="42" t="n">
-        <v>35.015155</v>
+        <v>-68.152733</v>
       </c>
       <c r="I66" s="45" t="n">
-        <v>34.17027197260274</v>
+        <v>-68.57462442307693</v>
       </c>
       <c r="J66" s="44" t="n">
-        <v>27.662124</v>
+        <v>-68.940006</v>
       </c>
       <c r="K66" s="42" t="n">
-        <v>35.015155</v>
+        <v>-68.06532799999999</v>
       </c>
       <c r="L66" s="45" t="n">
-        <v>32.47510082</v>
+        <v>-68.46212181764706</v>
       </c>
       <c r="M66" s="44" t="n">
-        <v>24.075044</v>
+        <v>-68.940006</v>
       </c>
       <c r="N66" s="42" t="n">
-        <v>35.015155</v>
+        <v>-67.715525</v>
       </c>
       <c r="O66" s="45" t="n">
-        <v>28.02186313436123</v>
+        <v>-68.32639864752475</v>
       </c>
       <c r="P66" s="92" t="n">
-        <v>14.764</v>
+        <v>3.36199</v>
       </c>
       <c r="Q66" s="91" t="n"/>
       <c r="R66" s="1" t="n"/>
@@ -7326,45 +7325,45 @@
       <c r="B67" s="16" t="n"/>
       <c r="C67" s="90" t="inlineStr">
         <is>
-          <t>Z1</t>
+          <t>SILT-TRAP</t>
         </is>
       </c>
       <c r="D67" s="91" t="n"/>
       <c r="E67" s="90" t="inlineStr">
         <is>
-          <t>VW-ZC-01</t>
+          <t>VW-28</t>
         </is>
       </c>
       <c r="F67" s="91" t="n"/>
       <c r="G67" s="44" t="n">
-        <v>-6.894296</v>
+        <v>22.431062</v>
       </c>
       <c r="H67" s="42" t="n">
-        <v>-6.158052</v>
+        <v>23.219117</v>
       </c>
       <c r="I67" s="45" t="n">
-        <v>-6.55188046835443</v>
+        <v>22.81069283333333</v>
       </c>
       <c r="J67" s="44" t="n">
-        <v>-6.894296</v>
+        <v>22.431062</v>
       </c>
       <c r="K67" s="42" t="n">
-        <v>-5.604612</v>
+        <v>23.394634</v>
       </c>
       <c r="L67" s="45" t="n">
-        <v>-6.314889752941177</v>
+        <v>22.84586545882353</v>
       </c>
       <c r="M67" s="44" t="n">
-        <v>-6.894296</v>
+        <v>21.905833</v>
       </c>
       <c r="N67" s="42" t="n">
-        <v>-3.206967</v>
+        <v>23.394634</v>
       </c>
       <c r="O67" s="45" t="n">
-        <v>-5.187005159844055</v>
+        <v>22.63979281386139</v>
       </c>
       <c r="P67" s="92" t="n">
-        <v>8.31</v>
+        <v>16.15899</v>
       </c>
       <c r="Q67" s="91" t="n"/>
       <c r="R67" s="1" t="n"/>
@@ -7382,39 +7381,39 @@
       <c r="D68" s="91" t="n"/>
       <c r="E68" s="90" t="inlineStr">
         <is>
-          <t>VW-27</t>
+          <t>VW-25</t>
         </is>
       </c>
       <c r="F68" s="91" t="n"/>
       <c r="G68" s="44" t="n">
-        <v>-68.765316</v>
+        <v>59.713098</v>
       </c>
       <c r="H68" s="42" t="n">
-        <v>-68.06532799999999</v>
+        <v>60.244496</v>
       </c>
       <c r="I68" s="45" t="n">
-        <v>-68.3909005443038</v>
+        <v>59.97331723076923</v>
       </c>
       <c r="J68" s="44" t="n">
-        <v>-68.765316</v>
+        <v>59.713098</v>
       </c>
       <c r="K68" s="42" t="n">
-        <v>-67.715525</v>
+        <v>60.508379</v>
       </c>
       <c r="L68" s="45" t="n">
-        <v>-68.29156432544379</v>
+        <v>60.05491837647059</v>
       </c>
       <c r="M68" s="44" t="n">
-        <v>-68.83043000000001</v>
+        <v>59.713098</v>
       </c>
       <c r="N68" s="42" t="n">
-        <v>-67.715525</v>
+        <v>60.774613</v>
       </c>
       <c r="O68" s="45" t="n">
-        <v>-68.32833769539079</v>
+        <v>60.14790612277228</v>
       </c>
       <c r="P68" s="92" t="n">
-        <v>3.36199</v>
+        <v>23.78799</v>
       </c>
       <c r="Q68" s="91" t="n"/>
       <c r="R68" s="1" t="n"/>
@@ -7426,45 +7425,45 @@
       <c r="B69" s="16" t="n"/>
       <c r="C69" s="90" t="inlineStr">
         <is>
-          <t>SILT-TRAP</t>
+          <t>Z1</t>
         </is>
       </c>
       <c r="D69" s="91" t="n"/>
       <c r="E69" s="90" t="inlineStr">
         <is>
-          <t>VW-28</t>
+          <t>Z1-4</t>
         </is>
       </c>
       <c r="F69" s="91" t="n"/>
       <c r="G69" s="44" t="n">
-        <v>22.431108</v>
+        <v>15.935861</v>
       </c>
       <c r="H69" s="42" t="n">
-        <v>23.394634</v>
+        <v>18.26053</v>
       </c>
       <c r="I69" s="45" t="n">
-        <v>22.95991470886076</v>
+        <v>17.04595600424328</v>
       </c>
       <c r="J69" s="44" t="n">
-        <v>22.431062</v>
+        <v>15.935861</v>
       </c>
       <c r="K69" s="42" t="n">
-        <v>23.394634</v>
+        <v>19.245763</v>
       </c>
       <c r="L69" s="45" t="n">
-        <v>22.90579028402367</v>
+        <v>17.69726002789116</v>
       </c>
       <c r="M69" s="44" t="n">
-        <v>22.04366</v>
+        <v>15.935861</v>
       </c>
       <c r="N69" s="42" t="n">
-        <v>23.394634</v>
+        <v>32.126094</v>
       </c>
       <c r="O69" s="45" t="n">
-        <v>22.63565579559118</v>
+        <v>19.05637021766457</v>
       </c>
       <c r="P69" s="92" t="n">
-        <v>16.15899</v>
+        <v>32.325</v>
       </c>
       <c r="Q69" s="91" t="n"/>
       <c r="R69" s="1" t="n"/>
@@ -7476,45 +7475,45 @@
       <c r="B70" s="16" t="n"/>
       <c r="C70" s="90" t="inlineStr">
         <is>
-          <t>SILT-TRAP</t>
+          <t>E1/E2</t>
         </is>
       </c>
       <c r="D70" s="91" t="n"/>
       <c r="E70" s="90" t="inlineStr">
         <is>
-          <t>VW-25</t>
+          <t>E2-3</t>
         </is>
       </c>
       <c r="F70" s="91" t="n"/>
       <c r="G70" s="44" t="n">
-        <v>59.845961</v>
+        <v>-6.617414</v>
       </c>
       <c r="H70" s="42" t="n">
-        <v>60.507784</v>
+        <v>-6.292486</v>
       </c>
       <c r="I70" s="45" t="n">
-        <v>60.11280716455696</v>
+        <v>-6.42923550997151</v>
       </c>
       <c r="J70" s="44" t="n">
-        <v>59.845961</v>
+        <v>-6.650593</v>
       </c>
       <c r="K70" s="42" t="n">
-        <v>60.774613</v>
+        <v>-6.292486</v>
       </c>
       <c r="L70" s="45" t="n">
-        <v>60.21071039053255</v>
+        <v>-6.462443801365188</v>
       </c>
       <c r="M70" s="44" t="n">
-        <v>59.845961</v>
+        <v>-7.159235</v>
       </c>
       <c r="N70" s="42" t="n">
-        <v>60.774613</v>
+        <v>-6.292486</v>
       </c>
       <c r="O70" s="45" t="n">
-        <v>60.25588139478958</v>
+        <v>-6.657144697359029</v>
       </c>
       <c r="P70" s="92" t="n">
-        <v>23.78799</v>
+        <v>2</v>
       </c>
       <c r="Q70" s="91" t="n"/>
       <c r="R70" s="1" t="n"/>
@@ -7526,45 +7525,45 @@
       <c r="B71" s="16" t="n"/>
       <c r="C71" s="90" t="inlineStr">
         <is>
-          <t>Z1</t>
+          <t>Y3</t>
         </is>
       </c>
       <c r="D71" s="91" t="n"/>
       <c r="E71" s="90" t="inlineStr">
         <is>
-          <t>Z1-4</t>
+          <t>Y3-2</t>
         </is>
       </c>
       <c r="F71" s="91" t="n"/>
       <c r="G71" s="44" t="n">
-        <v>16.801367</v>
+        <v>101.327138</v>
       </c>
       <c r="H71" s="42" t="n">
-        <v>18.869996</v>
+        <v>110.478298</v>
       </c>
       <c r="I71" s="45" t="n">
-        <v>17.74900611694153</v>
+        <v>106.2761555641026</v>
       </c>
       <c r="J71" s="44" t="n">
-        <v>16.801367</v>
+        <v>81.172364</v>
       </c>
       <c r="K71" s="42" t="n">
-        <v>20.091932</v>
+        <v>110.478298</v>
       </c>
       <c r="L71" s="45" t="n">
-        <v>18.39753425768156</v>
+        <v>98.67839992682927</v>
       </c>
       <c r="M71" s="44" t="n">
-        <v>16.801367</v>
+        <v>79.132493</v>
       </c>
       <c r="N71" s="42" t="n">
-        <v>32.126094</v>
+        <v>110.478298</v>
       </c>
       <c r="O71" s="45" t="n">
-        <v>19.42659756917756</v>
+        <v>87.22017264999999</v>
       </c>
       <c r="P71" s="92" t="n">
-        <v>32.325</v>
+        <v>15.17999</v>
       </c>
       <c r="Q71" s="91" t="n"/>
       <c r="R71" s="1" t="n"/>
@@ -7576,45 +7575,45 @@
       <c r="B72" s="16" t="n"/>
       <c r="C72" s="93" t="inlineStr">
         <is>
-          <t>E1/E2</t>
+          <t>CROWN</t>
         </is>
       </c>
       <c r="D72" s="94" t="n"/>
       <c r="E72" s="93" t="inlineStr">
         <is>
-          <t>E2-3</t>
+          <t>VW-43</t>
         </is>
       </c>
       <c r="F72" s="94" t="n"/>
       <c r="G72" s="46" t="n">
-        <v>-6.650593</v>
+        <v>-16.02496</v>
       </c>
       <c r="H72" s="47" t="n">
-        <v>-6.296649</v>
+        <v>-15.477164</v>
       </c>
       <c r="I72" s="48" t="n">
-        <v>-6.466663064467766</v>
+        <v>-15.7180891286425</v>
       </c>
       <c r="J72" s="46" t="n">
-        <v>-6.657684</v>
+        <v>-16.025736</v>
       </c>
       <c r="K72" s="47" t="n">
-        <v>-6.296649</v>
+        <v>-15.201814</v>
       </c>
       <c r="L72" s="48" t="n">
-        <v>-6.478616034482759</v>
+        <v>-15.63226850786056</v>
       </c>
       <c r="M72" s="46" t="n">
-        <v>-7.163219</v>
+        <v>-16.714466</v>
       </c>
       <c r="N72" s="47" t="n">
-        <v>-6.296649</v>
+        <v>-15.201814</v>
       </c>
       <c r="O72" s="48" t="n">
-        <v>-6.710027676449188</v>
+        <v>-15.86352377291764</v>
       </c>
       <c r="P72" s="95" t="n">
-        <v>2</v>
+        <v>22.25199</v>
       </c>
       <c r="Q72" s="94" t="n"/>
       <c r="R72" s="1" t="n"/>
@@ -7622,435 +7621,407 @@
       <c r="T72" s="1" t="n"/>
       <c r="U72" s="17" t="n"/>
     </row>
-    <row r="73" ht="14.25" customHeight="1" thickBot="1" thickTop="1">
+    <row r="73" ht="16.5" customHeight="1" thickBot="1" thickTop="1">
       <c r="B73" s="16" t="n"/>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>Y3</t>
-        </is>
-      </c>
-      <c r="E73" s="1" t="inlineStr">
-        <is>
-          <t>Y3-2</t>
-        </is>
-      </c>
-      <c r="F73" s="1" t="n"/>
-      <c r="G73" s="1" t="n">
-        <v>92.41611</v>
-      </c>
-      <c r="H73" s="1" t="n">
-        <v>105.906467</v>
-      </c>
-      <c r="I73" s="1" t="n">
-        <v>99.94623734615385</v>
-      </c>
-      <c r="J73" s="1" t="n">
-        <v>80.90196400000001</v>
-      </c>
-      <c r="K73" s="1" t="n">
-        <v>105.906467</v>
-      </c>
-      <c r="L73" s="1" t="n">
-        <v>91.6046230479042</v>
-      </c>
-      <c r="M73" s="1" t="n">
-        <v>79.132493</v>
-      </c>
-      <c r="N73" s="1" t="n">
-        <v>105.906467</v>
-      </c>
-      <c r="O73" s="1" t="n">
-        <v>85.12112468674698</v>
-      </c>
-      <c r="P73" s="1" t="n">
-        <v>15.17999</v>
-      </c>
-      <c r="Q73" s="1" t="n"/>
+      <c r="C73" s="93" t="inlineStr">
+        <is>
+          <t>CROWN</t>
+        </is>
+      </c>
+      <c r="D73" s="94" t="n"/>
+      <c r="E73" s="93" t="inlineStr">
+        <is>
+          <t>VW-46</t>
+        </is>
+      </c>
+      <c r="F73" s="94" t="n"/>
+      <c r="G73" s="46" t="n">
+        <v>-23.250927</v>
+      </c>
+      <c r="H73" s="47" t="n">
+        <v>-22.607114</v>
+      </c>
+      <c r="I73" s="48" t="n">
+        <v>-22.95138151005747</v>
+      </c>
+      <c r="J73" s="46" t="n">
+        <v>-23.250927</v>
+      </c>
+      <c r="K73" s="47" t="n">
+        <v>-22.505945</v>
+      </c>
+      <c r="L73" s="48" t="n">
+        <v>-22.88575098461538</v>
+      </c>
+      <c r="M73" s="46" t="n">
+        <v>-23.295158</v>
+      </c>
+      <c r="N73" s="47" t="n">
+        <v>-22.428018</v>
+      </c>
+      <c r="O73" s="48" t="n">
+        <v>-22.88641650794027</v>
+      </c>
+      <c r="P73" s="95" t="n">
+        <v>24.078</v>
+      </c>
+      <c r="Q73" s="94" t="n"/>
       <c r="R73" s="1" t="n"/>
       <c r="S73" s="1" t="n"/>
       <c r="T73" s="1" t="n"/>
       <c r="U73" s="17" t="n"/>
     </row>
-    <row r="74" ht="21.75" customHeight="1" thickBot="1" thickTop="1">
-      <c r="B74" s="38" t="n"/>
-      <c r="C74" s="39" t="inlineStr">
+    <row r="74" ht="16.5" customHeight="1" thickBot="1" thickTop="1">
+      <c r="B74" s="16" t="n"/>
+      <c r="C74" s="93" t="inlineStr">
+        <is>
+          <t>SILT-TRAP</t>
+        </is>
+      </c>
+      <c r="D74" s="94" t="n"/>
+      <c r="E74" s="93" t="inlineStr">
+        <is>
+          <t>VW-ST-05</t>
+        </is>
+      </c>
+      <c r="F74" s="94" t="n"/>
+      <c r="G74" s="46" t="n">
+        <v>23.531328</v>
+      </c>
+      <c r="H74" s="47" t="n">
+        <v>24.297658</v>
+      </c>
+      <c r="I74" s="48" t="n">
+        <v>23.8727993452381</v>
+      </c>
+      <c r="J74" s="46" t="n">
+        <v>23.531328</v>
+      </c>
+      <c r="K74" s="47" t="n">
+        <v>24.488794</v>
+      </c>
+      <c r="L74" s="48" t="n">
+        <v>23.96867740243902</v>
+      </c>
+      <c r="M74" s="46" t="n">
+        <v>23.531328</v>
+      </c>
+      <c r="N74" s="47" t="n">
+        <v>24.679922</v>
+      </c>
+      <c r="O74" s="48" t="n">
+        <v>24.16870211205074</v>
+      </c>
+      <c r="P74" s="95" t="n">
+        <v>44.018</v>
+      </c>
+      <c r="Q74" s="94" t="n"/>
+      <c r="U74" s="17" t="n"/>
+    </row>
+    <row r="75" ht="16.5" customHeight="1" thickBot="1" thickTop="1">
+      <c r="B75" s="16" t="n"/>
+      <c r="C75" s="93" t="inlineStr">
+        <is>
+          <t>SILT-TRAP</t>
+        </is>
+      </c>
+      <c r="D75" s="94" t="n"/>
+      <c r="E75" s="93" t="inlineStr">
+        <is>
+          <t>VW-ST-07</t>
+        </is>
+      </c>
+      <c r="F75" s="94" t="n"/>
+      <c r="G75" s="46" t="n">
+        <v>-9.540531</v>
+      </c>
+      <c r="H75" s="47" t="n">
+        <v>-8.386813</v>
+      </c>
+      <c r="I75" s="48" t="n">
+        <v>-8.970712903614459</v>
+      </c>
+      <c r="J75" s="46" t="n">
+        <v>-9.540531</v>
+      </c>
+      <c r="K75" s="47" t="n">
+        <v>-8.373886000000001</v>
+      </c>
+      <c r="L75" s="48" t="n">
+        <v>-8.885557676136363</v>
+      </c>
+      <c r="M75" s="46" t="n">
+        <v>-9.540531</v>
+      </c>
+      <c r="N75" s="47" t="n">
+        <v>-7.989393</v>
+      </c>
+      <c r="O75" s="48" t="n">
+        <v>-8.922269590196079</v>
+      </c>
+      <c r="P75" s="95" t="n">
+        <v>23.11199</v>
+      </c>
+      <c r="Q75" s="94" t="n"/>
+      <c r="U75" s="17" t="n"/>
+    </row>
+    <row r="76" ht="16.5" customHeight="1" thickBot="1" thickTop="1">
+      <c r="B76" s="16" t="n"/>
+      <c r="C76" s="93" t="inlineStr">
+        <is>
+          <t>RDS</t>
+        </is>
+      </c>
+      <c r="D76" s="94" t="n"/>
+      <c r="E76" s="93" t="inlineStr">
+        <is>
+          <t>VW-RDS-01</t>
+        </is>
+      </c>
+      <c r="F76" s="94" t="n"/>
+      <c r="G76" s="46" t="n">
+        <v>-11.662848</v>
+      </c>
+      <c r="H76" s="47" t="n">
+        <v>-10.882253</v>
+      </c>
+      <c r="I76" s="48" t="n">
+        <v>-11.32198636</v>
+      </c>
+      <c r="J76" s="46" t="n">
+        <v>-11.662848</v>
+      </c>
+      <c r="K76" s="47" t="n">
+        <v>-10.882111</v>
+      </c>
+      <c r="L76" s="48" t="n">
+        <v>-11.2675055448718</v>
+      </c>
+      <c r="M76" s="46" t="n">
+        <v>-13.421556</v>
+      </c>
+      <c r="N76" s="47" t="n">
+        <v>-10.88194</v>
+      </c>
+      <c r="O76" s="48" t="n">
+        <v>-11.58792066382979</v>
+      </c>
+      <c r="P76" s="95" t="n">
+        <v>34.82999</v>
+      </c>
+      <c r="Q76" s="94" t="n"/>
+      <c r="U76" s="17" t="n"/>
+    </row>
+    <row r="77" ht="16.5" customHeight="1" thickBot="1" thickTop="1">
+      <c r="B77" s="16" t="n"/>
+      <c r="C77" s="93" t="inlineStr">
+        <is>
+          <t>Y3</t>
+        </is>
+      </c>
+      <c r="D77" s="94" t="n"/>
+      <c r="E77" s="93" t="inlineStr">
+        <is>
+          <t>Y3-4</t>
+        </is>
+      </c>
+      <c r="F77" s="94" t="n"/>
+      <c r="G77" s="46" t="n">
+        <v>-83.141161</v>
+      </c>
+      <c r="H77" s="47" t="n">
+        <v>-71.848867</v>
+      </c>
+      <c r="I77" s="48" t="n">
+        <v>-77.02232091025641</v>
+      </c>
+      <c r="J77" s="46" t="n">
+        <v>-90.91748800000001</v>
+      </c>
+      <c r="K77" s="47" t="n">
+        <v>-71.848867</v>
+      </c>
+      <c r="L77" s="48" t="n">
+        <v>-82.67229529878048</v>
+      </c>
+      <c r="M77" s="46" t="n">
+        <v>-98.85283800000001</v>
+      </c>
+      <c r="N77" s="47" t="n">
+        <v>-71.848867</v>
+      </c>
+      <c r="O77" s="48" t="n">
+        <v>-87.239651838</v>
+      </c>
+      <c r="P77" s="95" t="n">
+        <v>6.37999</v>
+      </c>
+      <c r="Q77" s="94" t="n"/>
+      <c r="U77" s="17" t="n"/>
+    </row>
+    <row r="78" ht="16.5" customHeight="1" thickBot="1" thickTop="1">
+      <c r="B78" s="16" t="n"/>
+      <c r="C78" s="93" t="inlineStr">
+        <is>
+          <t>Y3</t>
+        </is>
+      </c>
+      <c r="D78" s="94" t="n"/>
+      <c r="E78" s="93" t="inlineStr">
+        <is>
+          <t>Y3-3</t>
+        </is>
+      </c>
+      <c r="F78" s="94" t="n"/>
+      <c r="G78" s="46" t="n">
+        <v>38.524843</v>
+      </c>
+      <c r="H78" s="47" t="n">
+        <v>50.036738</v>
+      </c>
+      <c r="I78" s="48" t="n">
+        <v>44.903176</v>
+      </c>
+      <c r="J78" s="46" t="n">
+        <v>15.743003</v>
+      </c>
+      <c r="K78" s="47" t="n">
+        <v>50.036738</v>
+      </c>
+      <c r="L78" s="48" t="n">
+        <v>35.93165967682927</v>
+      </c>
+      <c r="M78" s="46" t="n">
+        <v>-25.714093</v>
+      </c>
+      <c r="N78" s="47" t="n">
+        <v>50.036738</v>
+      </c>
+      <c r="O78" s="48" t="n">
+        <v>4.88093702</v>
+      </c>
+      <c r="P78" s="95" t="n">
+        <v>5.77999</v>
+      </c>
+      <c r="Q78" s="94" t="n"/>
+      <c r="U78" s="17" t="n"/>
+    </row>
+    <row r="79" ht="16.5" customHeight="1" thickBot="1" thickTop="1">
+      <c r="B79" s="16" t="n"/>
+      <c r="C79" s="93" t="inlineStr">
         <is>
           <t>CROWN</t>
         </is>
       </c>
-      <c r="D74" s="39" t="n"/>
-      <c r="E74" s="39" t="inlineStr">
-        <is>
-          <t>VW-43</t>
-        </is>
-      </c>
-      <c r="F74" s="39" t="n"/>
-      <c r="G74" s="39" t="n">
-        <v>-16.025736</v>
-      </c>
-      <c r="H74" s="39" t="n">
-        <v>-15.478288</v>
-      </c>
-      <c r="I74" s="39" t="n">
-        <v>-15.75170457712566</v>
-      </c>
-      <c r="J74" s="39" t="n">
-        <v>-16.025736</v>
-      </c>
-      <c r="K74" s="39" t="n">
-        <v>-15.201814</v>
-      </c>
-      <c r="L74" s="39" t="n">
-        <v>-15.56971266970547</v>
-      </c>
-      <c r="M74" s="39" t="n">
-        <v>-16.987484</v>
-      </c>
-      <c r="N74" s="39" t="n">
-        <v>-15.201814</v>
-      </c>
-      <c r="O74" s="39" t="n">
-        <v>-15.95090926040062</v>
-      </c>
-      <c r="P74" s="39" t="n">
-        <v>22.25199</v>
-      </c>
-      <c r="Q74" s="39" t="n"/>
-      <c r="R74" s="39" t="n"/>
-      <c r="S74" s="39" t="n"/>
-      <c r="T74" s="39" t="n"/>
-      <c r="U74" s="40" t="n"/>
+      <c r="D79" s="94" t="n"/>
+      <c r="E79" s="93" t="inlineStr">
+        <is>
+          <t>VW-CN-03</t>
+        </is>
+      </c>
+      <c r="F79" s="94" t="n"/>
+      <c r="G79" s="46" t="n">
+        <v>71.90974900000001</v>
+      </c>
+      <c r="H79" s="47" t="n">
+        <v>73.17980799999999</v>
+      </c>
+      <c r="I79" s="48" t="n">
+        <v>72.50214657768362</v>
+      </c>
+      <c r="J79" s="46" t="n">
+        <v>70.929123</v>
+      </c>
+      <c r="K79" s="47" t="n">
+        <v>73.17980799999999</v>
+      </c>
+      <c r="L79" s="48" t="n">
+        <v>72.12594479065041</v>
+      </c>
+      <c r="M79" s="46" t="n">
+        <v>69.033439</v>
+      </c>
+      <c r="N79" s="47" t="n">
+        <v>73.17980799999999</v>
+      </c>
+      <c r="O79" s="48" t="n">
+        <v>71.26365571192053</v>
+      </c>
+      <c r="P79" s="95" t="n">
+        <v>51.71999</v>
+      </c>
+      <c r="Q79" s="94" t="n"/>
+      <c r="U79" s="17" t="n"/>
     </row>
-    <row r="75" ht="13.5" customHeight="1" thickTop="1">
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>CROWN</t>
-        </is>
-      </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>VW-46</t>
-        </is>
-      </c>
-      <c r="G75" t="n">
-        <v>-23.094261</v>
-      </c>
-      <c r="H75" t="n">
-        <v>-22.505945</v>
-      </c>
-      <c r="I75" t="n">
-        <v>-22.78397241068702</v>
-      </c>
-      <c r="J75" t="n">
-        <v>-23.094261</v>
-      </c>
-      <c r="K75" t="n">
-        <v>-22.428018</v>
-      </c>
-      <c r="L75" t="n">
-        <v>-22.77642881681034</v>
-      </c>
-      <c r="M75" t="n">
-        <v>-23.20595</v>
-      </c>
-      <c r="N75" t="n">
-        <v>-22.428018</v>
-      </c>
-      <c r="O75" t="n">
-        <v>-22.84405101692866</v>
-      </c>
-      <c r="P75" t="n">
-        <v>24.078</v>
-      </c>
+    <row r="80" ht="14.25" customHeight="1" thickBot="1" thickTop="1">
+      <c r="B80" s="16" t="n"/>
+      <c r="U80" s="17" t="n"/>
     </row>
-    <row r="76">
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>SILT-TRAP</t>
-        </is>
-      </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>VW-ST-05</t>
-        </is>
-      </c>
-      <c r="G76" t="n">
-        <v>23.722499</v>
-      </c>
-      <c r="H76" t="n">
-        <v>24.488681</v>
-      </c>
-      <c r="I76" t="n">
-        <v>24.06898943243243</v>
-      </c>
-      <c r="J76" t="n">
-        <v>23.722499</v>
-      </c>
-      <c r="K76" t="n">
-        <v>24.67985</v>
-      </c>
-      <c r="L76" t="n">
-        <v>24.12967256687898</v>
-      </c>
-      <c r="M76" t="n">
-        <v>23.722499</v>
-      </c>
-      <c r="N76" t="n">
-        <v>24.679922</v>
-      </c>
-      <c r="O76" t="n">
-        <v>24.23949097603486</v>
-      </c>
-      <c r="P76" t="n">
-        <v>44.018</v>
-      </c>
+    <row r="81" ht="21.75" customHeight="1" thickBot="1" thickTop="1">
+      <c r="B81" s="38" t="n"/>
+      <c r="C81" s="39" t="n"/>
+      <c r="D81" s="39" t="n"/>
+      <c r="E81" s="39" t="n"/>
+      <c r="F81" s="39" t="n"/>
+      <c r="G81" s="39" t="n"/>
+      <c r="H81" s="39" t="n"/>
+      <c r="I81" s="39" t="n"/>
+      <c r="J81" s="39" t="n"/>
+      <c r="K81" s="39" t="n"/>
+      <c r="L81" s="39" t="n"/>
+      <c r="M81" s="39" t="n"/>
+      <c r="N81" s="39" t="n"/>
+      <c r="O81" s="39" t="n"/>
+      <c r="P81" s="39" t="n"/>
+      <c r="Q81" s="39" t="n"/>
+      <c r="R81" s="39" t="n"/>
+      <c r="S81" s="39" t="n"/>
+      <c r="T81" s="39" t="n"/>
+      <c r="U81" s="40" t="n"/>
     </row>
-    <row r="77">
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>SILT-TRAP</t>
-        </is>
-      </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>VW-ST-07</t>
-        </is>
-      </c>
-      <c r="G77" t="n">
-        <v>-9.333107</v>
-      </c>
-      <c r="H77" t="n">
-        <v>-8.374101</v>
-      </c>
-      <c r="I77" t="n">
-        <v>-8.768381612500001</v>
-      </c>
-      <c r="J77" t="n">
-        <v>-9.342547</v>
-      </c>
-      <c r="K77" t="n">
-        <v>-7.989393</v>
-      </c>
-      <c r="L77" t="n">
-        <v>-8.787496976878613</v>
-      </c>
-      <c r="M77" t="n">
-        <v>-9.612774999999999</v>
-      </c>
-      <c r="N77" t="n">
-        <v>-7.989393</v>
-      </c>
-      <c r="O77" t="n">
-        <v>-8.943656757999999</v>
-      </c>
-      <c r="P77" t="n">
-        <v>23.11199</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>RDS</t>
-        </is>
-      </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>VW-RDS-01</t>
-        </is>
-      </c>
-      <c r="G78" t="n">
-        <v>-11.467535</v>
-      </c>
-      <c r="H78" t="n">
-        <v>-10.882253</v>
-      </c>
-      <c r="I78" t="n">
-        <v>-11.18150602666667</v>
-      </c>
-      <c r="J78" t="n">
-        <v>-11.467564</v>
-      </c>
-      <c r="K78" t="n">
-        <v>-10.882076</v>
-      </c>
-      <c r="L78" t="n">
-        <v>-11.17363268181818</v>
-      </c>
-      <c r="M78" t="n">
-        <v>-13.421556</v>
-      </c>
-      <c r="N78" t="n">
-        <v>-10.88194</v>
-      </c>
-      <c r="O78" t="n">
-        <v>-11.71581479310345</v>
-      </c>
-      <c r="P78" t="n">
-        <v>34.82999</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>Y3</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>Y3-4</t>
-        </is>
-      </c>
-      <c r="G79" t="n">
-        <v>-90.91748800000001</v>
-      </c>
-      <c r="H79" t="n">
-        <v>-77.55825400000001</v>
-      </c>
-      <c r="I79" t="n">
-        <v>-84.45196353846154</v>
-      </c>
-      <c r="J79" t="n">
-        <v>-90.91748800000001</v>
-      </c>
-      <c r="K79" t="n">
-        <v>-77.55825400000001</v>
-      </c>
-      <c r="L79" t="n">
-        <v>-85.7486847245509</v>
-      </c>
-      <c r="M79" t="n">
-        <v>-99.235359</v>
-      </c>
-      <c r="N79" t="n">
-        <v>-77.55825400000001</v>
-      </c>
-      <c r="O79" t="n">
-        <v>-89.29935552008033</v>
-      </c>
-      <c r="P79" t="n">
-        <v>6.37999</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>Y3</t>
-        </is>
-      </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>Y3-3</t>
-        </is>
-      </c>
-      <c r="G80" t="n">
-        <v>28.135323</v>
-      </c>
-      <c r="H80" t="n">
-        <v>44.34952</v>
-      </c>
-      <c r="I80" t="n">
-        <v>37.0694822051282</v>
-      </c>
-      <c r="J80" t="n">
-        <v>2.651223</v>
-      </c>
-      <c r="K80" t="n">
-        <v>44.34952</v>
-      </c>
-      <c r="L80" t="n">
-        <v>25.48164258083832</v>
-      </c>
-      <c r="M80" t="n">
-        <v>-25.401467</v>
-      </c>
-      <c r="N80" t="n">
-        <v>44.34952</v>
-      </c>
-      <c r="O80" t="n">
-        <v>-0.9161741746987951</v>
-      </c>
-      <c r="P80" t="n">
-        <v>5.77999</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>CROWN</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>VW-CN-03</t>
-        </is>
-      </c>
-      <c r="G81" t="n">
-        <v>71.41374</v>
-      </c>
-      <c r="H81" t="n">
-        <v>72.821449</v>
-      </c>
-      <c r="I81" t="n">
-        <v>72.15042007749628</v>
-      </c>
-      <c r="J81" t="n">
-        <v>70.458822</v>
-      </c>
-      <c r="K81" t="n">
-        <v>72.821449</v>
-      </c>
-      <c r="L81" t="n">
-        <v>71.73985189902507</v>
-      </c>
-      <c r="M81" t="n">
-        <v>69.033439</v>
-      </c>
-      <c r="N81" t="n">
-        <v>72.821449</v>
-      </c>
-      <c r="O81" t="n">
-        <v>71.05047816237014</v>
-      </c>
-      <c r="P81" t="n">
-        <v>51.71999</v>
-      </c>
-    </row>
+    <row r="82" ht="13.5" customHeight="1" thickTop="1"/>
   </sheetData>
-  <mergeCells count="192">
+  <mergeCells count="213">
     <mergeCell ref="C62:D62"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="P76:Q76"/>
     <mergeCell ref="C15:D15"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="E62:F62"/>
     <mergeCell ref="E71:F71"/>
     <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C64:D64"/>
     <mergeCell ref="M12:O12"/>
     <mergeCell ref="P69:Q69"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="E79:F79"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="E73:F73"/>
     <mergeCell ref="E64:F64"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="E51:F51"/>
     <mergeCell ref="P12:Q13"/>
-    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="C73:D73"/>
     <mergeCell ref="C54:D54"/>
     <mergeCell ref="P59:Q59"/>
     <mergeCell ref="C63:D63"/>
     <mergeCell ref="C41:D41"/>
+    <mergeCell ref="P46:Q46"/>
     <mergeCell ref="E63:F63"/>
-    <mergeCell ref="P46:Q46"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="C56:D56"/>
     <mergeCell ref="P61:Q61"/>
+    <mergeCell ref="P39:Q39"/>
     <mergeCell ref="E65:F65"/>
-    <mergeCell ref="P39:Q39"/>
+    <mergeCell ref="P70:Q70"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="P48:Q48"/>
     <mergeCell ref="C43:D43"/>
-    <mergeCell ref="P48:Q48"/>
-    <mergeCell ref="P70:Q70"/>
-    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="P32:Q32"/>
     <mergeCell ref="E49:F49"/>
-    <mergeCell ref="P32:Q32"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C27:D27"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="P47:Q47"/>
@@ -8059,12 +8030,15 @@
     <mergeCell ref="P15:Q15"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="P58:Q58"/>
+    <mergeCell ref="P33:Q33"/>
+    <mergeCell ref="E53:F53"/>
     <mergeCell ref="C28:D28"/>
-    <mergeCell ref="P33:Q33"/>
     <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="P58:Q58"/>
     <mergeCell ref="C69:D69"/>
+    <mergeCell ref="P79:Q79"/>
+    <mergeCell ref="P73:Q73"/>
     <mergeCell ref="M11:O11"/>
     <mergeCell ref="P26:Q26"/>
     <mergeCell ref="C12:D13"/>
@@ -8073,11 +8047,11 @@
     <mergeCell ref="E55:F55"/>
     <mergeCell ref="P63:Q63"/>
     <mergeCell ref="E67:F67"/>
-    <mergeCell ref="C14:D14"/>
     <mergeCell ref="C45:D45"/>
+    <mergeCell ref="P50:Q50"/>
     <mergeCell ref="P25:Q25"/>
     <mergeCell ref="E14:F14"/>
-    <mergeCell ref="P50:Q50"/>
+    <mergeCell ref="C14:D14"/>
     <mergeCell ref="E48:F48"/>
     <mergeCell ref="P60:Q60"/>
     <mergeCell ref="P34:Q34"/>
@@ -8087,13 +8061,16 @@
     <mergeCell ref="P36:Q36"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="E40:F40"/>
+    <mergeCell ref="P77:Q77"/>
     <mergeCell ref="C60:D60"/>
     <mergeCell ref="M4:O4"/>
     <mergeCell ref="C71:D71"/>
     <mergeCell ref="P28:Q28"/>
     <mergeCell ref="P37:Q37"/>
     <mergeCell ref="E26:F26"/>
+    <mergeCell ref="P78:Q78"/>
     <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E76:F76"/>
     <mergeCell ref="P30:Q30"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="C57:D57"/>
@@ -8104,61 +8081,66 @@
     <mergeCell ref="E66:F66"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C53:D53"/>
+    <mergeCell ref="E58:F58"/>
     <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E58:F58"/>
     <mergeCell ref="P55:Q55"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="E50:F50"/>
     <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E50:F50"/>
     <mergeCell ref="P64:Q64"/>
     <mergeCell ref="C68:D68"/>
+    <mergeCell ref="P51:Q51"/>
+    <mergeCell ref="E68:F68"/>
     <mergeCell ref="D3:J3"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="P51:Q51"/>
     <mergeCell ref="C58:D58"/>
     <mergeCell ref="E52:F52"/>
     <mergeCell ref="P41:Q41"/>
     <mergeCell ref="E39:F39"/>
     <mergeCell ref="E44:F44"/>
     <mergeCell ref="C20:D20"/>
+    <mergeCell ref="P56:Q56"/>
+    <mergeCell ref="C29:D29"/>
     <mergeCell ref="E20:F20"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="P56:Q56"/>
     <mergeCell ref="E29:F29"/>
     <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C75:D75"/>
     <mergeCell ref="P49:Q49"/>
-    <mergeCell ref="B2:U2"/>
-    <mergeCell ref="C22:D22"/>
     <mergeCell ref="E69:F69"/>
     <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="P67:Q67"/>
     <mergeCell ref="C31:D31"/>
-    <mergeCell ref="P67:Q67"/>
     <mergeCell ref="E31:F31"/>
+    <mergeCell ref="B2:U2"/>
     <mergeCell ref="C59:D59"/>
     <mergeCell ref="M5:P5"/>
     <mergeCell ref="E59:F59"/>
     <mergeCell ref="P17:Q17"/>
     <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E77:F77"/>
     <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E46:F46"/>
     <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E46:F46"/>
     <mergeCell ref="C51:D51"/>
     <mergeCell ref="C61:D61"/>
     <mergeCell ref="P66:Q66"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="P75:Q75"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="P53:Q53"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="C48:D48"/>
     <mergeCell ref="G12:I12"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="E61:F61"/>
-    <mergeCell ref="C48:D48"/>
     <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="P53:Q53"/>
     <mergeCell ref="E57:F57"/>
     <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E54:F54"/>
     <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="P68:Q68"/>
     <mergeCell ref="E32:F32"/>
-    <mergeCell ref="P68:Q68"/>
     <mergeCell ref="E72:F72"/>
     <mergeCell ref="E41:F41"/>
     <mergeCell ref="B6:U6"/>
@@ -8175,6 +8157,7 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="C42:D42"/>
     <mergeCell ref="E42:F42"/>
+    <mergeCell ref="C74:D74"/>
     <mergeCell ref="P44:Q44"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="C26:D26"/>
@@ -8190,12 +8173,13 @@
     <mergeCell ref="C55:D55"/>
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="P65:Q65"/>
+    <mergeCell ref="E60:F60"/>
     <mergeCell ref="J12:L12"/>
-    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="E74:F74"/>
     <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="S5:U5"/>
     <mergeCell ref="E12:F13"/>
     <mergeCell ref="E30:F30"/>
+    <mergeCell ref="S5:U5"/>
     <mergeCell ref="P16:Q16"/>
     <mergeCell ref="E45:F45"/>
     <mergeCell ref="C52:D52"/>
@@ -8207,6 +8191,8 @@
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="P42:Q42"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="P74:Q74"/>
+    <mergeCell ref="C78:D78"/>
     <mergeCell ref="E47:F47"/>
     <mergeCell ref="E21:F21"/>
   </mergeCells>

</xml_diff>